<commit_message>
creating parametric survival parameters for individual arms, stacking those for into a bugs data set and running multivariate NMA
</commit_message>
<xml_diff>
--- a/Data/bugsdata/parametric survival bugs data.xlsx
+++ b/Data/bugsdata/parametric survival bugs data.xlsx
@@ -1260,25 +1260,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.39500202175584</v>
+        <v>-2.33006830871177</v>
       </c>
       <c r="F2" t="n">
-        <v>0.10812372759168</v>
+        <v>0.10533870155035</v>
       </c>
       <c r="G2" t="n">
-        <v>0.103772517733394</v>
+        <v>0.105924771630349</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0769739957034721</v>
+        <v>0.0881247958125287</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0116907404683198</v>
+        <v>0.0110962420443137</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00592499601455814</v>
+        <v>0.00776597963699988</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.00402251489432989</v>
+        <v>-0.00350576567788289</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -1298,25 +1298,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.57824772385901</v>
+        <v>-2.49972872840229</v>
       </c>
       <c r="F3" t="n">
-        <v>0.125256517287666</v>
+        <v>0.122057447093382</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0468565894924138</v>
+        <v>0.0391414385130606</v>
       </c>
       <c r="H3" t="n">
-        <v>0.05928365352867</v>
+        <v>0.0517908396172799</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0156891951230354</v>
+        <v>0.0148980203909537</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00351455157570738</v>
+        <v>0.00268229106826281</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.00425682222495584</v>
+        <v>-0.00257155016007909</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -1336,25 +1336,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.13810935882744</v>
+        <v>-3.09126802584416</v>
       </c>
       <c r="F4" t="n">
-        <v>0.188580141371055</v>
+        <v>0.175312283413101</v>
       </c>
       <c r="G4" t="n">
-        <v>0.150618291702876</v>
+        <v>0.143473106550909</v>
       </c>
       <c r="H4" t="n">
-        <v>0.122038959982672</v>
+        <v>0.117818399725227</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0355624697195271</v>
+        <v>0.0307343967155154</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0148935077536523</v>
+        <v>0.0138811753138134</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0152701894491901</v>
+        <v>-0.0141763938303875</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -1374,25 +1374,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>-3.58822680878078</v>
+        <v>-3.48734749630726</v>
       </c>
       <c r="F5" t="n">
-        <v>0.250481693413968</v>
+        <v>0.242367660737922</v>
       </c>
       <c r="G5" t="n">
-        <v>0.327498708634429</v>
+        <v>0.282416396265322</v>
       </c>
       <c r="H5" t="n">
-        <v>0.118770393218704</v>
+        <v>0.11231437447069</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0627410787355289</v>
+        <v>0.0587420829715727</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0141064063053257</v>
+        <v>0.0126145187127423</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0232967607253938</v>
+        <v>-0.0229317679615367</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -1412,25 +1412,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.48739851639861</v>
+        <v>-2.41945335488241</v>
       </c>
       <c r="F6" t="n">
-        <v>0.119237197740365</v>
+        <v>0.107605083706125</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0173439251044164</v>
+        <v>-0.0399294119806398</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0858621209145547</v>
+        <v>0.0802228258285359</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0142175093249749</v>
+        <v>0.0115788540394022</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00737230380794561</v>
+        <v>0.00643570178391561</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.00675677729281162</v>
+        <v>-0.00318512887970389</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -1450,25 +1450,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.61351770303824</v>
+        <v>-2.56891849151363</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0912646059721666</v>
+        <v>0.0953207574839895</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0447916602245716</v>
+        <v>-0.0434775808987697</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0750187544228287</v>
+        <v>0.101936547928577</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00832922830325483</v>
+        <v>0.00908604680732155</v>
       </c>
       <c r="J7" t="n">
-        <v>0.00562781351515267</v>
+        <v>0.0103910598035951</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.00329069460677465</v>
+        <v>-0.00562530671538125</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -1488,25 +1488,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.35992376256339</v>
+        <v>-2.28927585322432</v>
       </c>
       <c r="F8" t="n">
-        <v>0.309719915328088</v>
+        <v>0.263546347264198</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.153144231507661</v>
+        <v>-0.107253607990594</v>
       </c>
       <c r="H8" t="n">
-        <v>0.150161873039823</v>
+        <v>0.169984735668374</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0959264259508379</v>
+        <v>0.0694566771563014</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0225485881148278</v>
+        <v>0.0288948103602471</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0218092681903502</v>
+        <v>-0.0143544642403251</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -1526,25 +1526,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-3.00978071494291</v>
+        <v>-2.97605246674702</v>
       </c>
       <c r="F9" t="n">
-        <v>0.294620451678279</v>
+        <v>0.323540867216825</v>
       </c>
       <c r="G9" t="n">
-        <v>0.138978900167005</v>
+        <v>0.137278719565766</v>
       </c>
       <c r="H9" t="n">
-        <v>0.170187449721332</v>
+        <v>0.216077907045135</v>
       </c>
       <c r="I9" t="n">
-        <v>0.086801210547113</v>
+        <v>0.104678692759415</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0289637680426511</v>
+        <v>0.0466896619130061</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0421769037283446</v>
+        <v>-0.0591706299533721</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -1564,25 +1564,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.14218267845162</v>
+        <v>-2.0472551672577</v>
       </c>
       <c r="F10" t="n">
-        <v>0.273912315481934</v>
+        <v>0.261938085818681</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1969390943671</v>
+        <v>0.155430830791449</v>
       </c>
       <c r="H10" t="n">
-        <v>0.161633137077179</v>
+        <v>0.172266877897778</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0750279565726748</v>
+        <v>0.0686115608023547</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0261252710014103</v>
+        <v>0.0296758772206481</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0311812098035073</v>
+        <v>-0.0339121655313017</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -1602,25 +1602,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.82367267232602</v>
+        <v>-2.6879308622404</v>
       </c>
       <c r="F11" t="n">
-        <v>0.324682196980101</v>
+        <v>0.254893879407089</v>
       </c>
       <c r="G11" t="n">
-        <v>0.175621856814685</v>
+        <v>0.130167622053188</v>
       </c>
       <c r="H11" t="n">
-        <v>0.13578283802204</v>
+        <v>0.11158061989941</v>
       </c>
       <c r="I11" t="n">
-        <v>0.105418529035825</v>
+        <v>0.0649708897591956</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0184369791013194</v>
+        <v>0.0124502347371367</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0377651881515243</v>
+        <v>-0.0206858569923194</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -1640,25 +1640,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.85084742220134</v>
+        <v>-2.76488446758512</v>
       </c>
       <c r="F12" t="n">
-        <v>0.373118632041817</v>
+        <v>0.2959383108534</v>
       </c>
       <c r="G12" t="n">
-        <v>0.191139707450786</v>
+        <v>0.174964827340232</v>
       </c>
       <c r="H12" t="n">
-        <v>0.184639301058125</v>
+        <v>0.114840037842542</v>
       </c>
       <c r="I12" t="n">
-        <v>0.139217513576757</v>
+        <v>0.0875794838307637</v>
       </c>
       <c r="J12" t="n">
-        <v>0.034091671495233</v>
+        <v>0.0131882342916765</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0563951175806997</v>
+        <v>-0.0198566769345156</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -1678,25 +1678,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>-4.00779465950803</v>
+        <v>-3.92419203737332</v>
       </c>
       <c r="F13" t="n">
-        <v>0.628093159789506</v>
+        <v>0.494772230509085</v>
       </c>
       <c r="G13" t="n">
-        <v>0.375222007563247</v>
+        <v>0.360426783558681</v>
       </c>
       <c r="H13" t="n">
-        <v>0.244402793342619</v>
+        <v>0.187127507302931</v>
       </c>
       <c r="I13" t="n">
-        <v>0.394501017374366</v>
+        <v>0.244799560082935</v>
       </c>
       <c r="J13" t="n">
-        <v>0.059732725393675</v>
+        <v>0.0350167039894086</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.14457190032534</v>
+        <v>-0.0810677652745029</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -1716,25 +1716,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>-2.84402157787172</v>
+        <v>-2.79738339481437</v>
       </c>
       <c r="F14" t="n">
-        <v>0.166400404319523</v>
+        <v>0.171698196289065</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0114217344621236</v>
+        <v>-0.0139801110920569</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0918101730715185</v>
+        <v>0.105889677952872</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0276890945577009</v>
+        <v>0.0294802706089184</v>
       </c>
       <c r="J14" t="n">
-        <v>0.00842910787942218</v>
+        <v>0.011212623896963</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.00936032305604423</v>
+        <v>-0.0116199924086907</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -1754,25 +1754,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>-3.01920941114309</v>
+        <v>-2.95410791709162</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1957543823296</v>
+        <v>0.173133254677496</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0688710722139505</v>
+        <v>0.0556593266224006</v>
       </c>
       <c r="H15" t="n">
-        <v>0.106918285891009</v>
+        <v>0.0926145582214106</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0383197782012431</v>
+        <v>0.0299751238752225</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0114315198578715</v>
+        <v>0.00857745639454706</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.0153403431417579</v>
+        <v>-0.0112536040524681</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -1792,25 +1792,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.8473150791631</v>
+        <v>-2.79756053367509</v>
       </c>
       <c r="F16" t="n">
-        <v>0.144695958439284</v>
+        <v>0.119642980975563</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0750160783595377</v>
+        <v>-0.0884476008590871</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0858304841970044</v>
+        <v>0.0838583312620675</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0209369203886629</v>
+        <v>0.014314442896719</v>
       </c>
       <c r="J16" t="n">
-        <v>0.00736687201749222</v>
+        <v>0.00703221972205866</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.00586329307363494</v>
+        <v>-0.00234476540435095</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -1830,25 +1830,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.83658401006587</v>
+        <v>-1.8496768167544</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0953889499198419</v>
+        <v>0.0713815590614557</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.197722113791001</v>
+        <v>-0.201232123211273</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0419833442232253</v>
+        <v>0.036854147082554</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00909905176681011</v>
+        <v>0.00509532697404409</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00176260119216583</v>
+        <v>0.00135822815718253</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.000608601100755223</v>
+        <v>-0.000288346995536712</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -1868,25 +1868,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>-2.02920667547382</v>
+        <v>-2.04690973252514</v>
       </c>
       <c r="F18" t="n">
-        <v>0.101386015116349</v>
+        <v>0.0737316968516354</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.165252558924571</v>
+        <v>-0.171946395700535</v>
       </c>
       <c r="H18" t="n">
-        <v>0.04858091302945</v>
+        <v>0.0388523711236188</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0102791240611726</v>
+        <v>0.00543636312062147</v>
       </c>
       <c r="J18" t="n">
-        <v>0.00236010511077498</v>
+        <v>0.00150950674192741</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.0018486256997203</v>
+        <v>-0.00158773213442984</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -1906,25 +1906,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.88701180933812</v>
+        <v>-2.83545108599723</v>
       </c>
       <c r="F19" t="n">
-        <v>0.187647325679811</v>
+        <v>0.159160874987795</v>
       </c>
       <c r="G19" t="n">
-        <v>0.161475571525528</v>
+        <v>0.145673114301433</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0969665892615014</v>
+        <v>0.0977476357725525</v>
       </c>
       <c r="I19" t="n">
-        <v>0.035211518834785</v>
+        <v>0.0253321841268806</v>
       </c>
       <c r="J19" t="n">
-        <v>0.00940251943300871</v>
+        <v>0.00955460029912358</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0137431723158013</v>
+        <v>-0.0120621687812353</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -1944,25 +1944,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.80076969518453</v>
+        <v>-2.72194870874295</v>
       </c>
       <c r="F20" t="n">
-        <v>0.199420834984694</v>
+        <v>0.163891712200428</v>
       </c>
       <c r="G20" t="n">
-        <v>0.300144465918335</v>
+        <v>0.255836150826446</v>
       </c>
       <c r="H20" t="n">
-        <v>0.135723151780683</v>
+        <v>0.118697956862633</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0397686694259927</v>
+        <v>0.026860493327988</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0184207739292822</v>
+        <v>0.0140892049633635</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0225109028945209</v>
+        <v>-0.0149839404293542</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -1982,25 +1982,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.95308165608033</v>
+        <v>-1.91600227134157</v>
       </c>
       <c r="F21" t="n">
-        <v>0.235764186065949</v>
+        <v>0.257928758189887</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.127807148941032</v>
+        <v>-0.139560850406393</v>
       </c>
       <c r="H21" t="n">
-        <v>0.128157101154197</v>
+        <v>0.105925170492656</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0555847514313396</v>
+        <v>0.0665272443013772</v>
       </c>
       <c r="J21" t="n">
-        <v>0.016424242576247</v>
+        <v>0.0112201417438982</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.014699123668472</v>
+        <v>-0.0112609082153799</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -2020,25 +2020,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>-2.70892943143692</v>
+        <v>-2.61515646363081</v>
       </c>
       <c r="F22" t="n">
-        <v>0.395908632478748</v>
+        <v>0.320756770614934</v>
       </c>
       <c r="G22" t="n">
-        <v>0.242382907798554</v>
+        <v>0.213278475676705</v>
       </c>
       <c r="H22" t="n">
-        <v>0.219530970391322</v>
+        <v>0.172728878584829</v>
       </c>
       <c r="I22" t="n">
-        <v>0.156743645271192</v>
+        <v>0.102884905895322</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0481938469609553</v>
+        <v>0.0298352654971725</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0662510125415888</v>
+        <v>-0.0348334841073863</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>
@@ -2110,25 +2110,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>2.03645638169679</v>
+        <v>1.97970353858253</v>
       </c>
       <c r="F2" t="n">
-        <v>0.152717764270313</v>
+        <v>0.145690465580844</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.12190166059483</v>
+        <v>-1.12832256940951</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0867906653867666</v>
+        <v>0.103194604784936</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0233227155237229</v>
+        <v>0.0212257117611632</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00753261959827769</v>
+        <v>0.0106491264567192</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.0107506639965146</v>
+        <v>-0.0124958410297487</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -2148,25 +2148,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>2.0046720337807</v>
+        <v>1.93563637872471</v>
       </c>
       <c r="F3" t="n">
-        <v>0.150216926418198</v>
+        <v>0.121436695299748</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.992824174200785</v>
+        <v>-0.991804474991053</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0678852275553906</v>
+        <v>0.0583512054430059</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0225651249825304</v>
+        <v>0.0147468709653237</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00460840412024716</v>
+        <v>0.00340486317665188</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.00802013418412126</v>
+        <v>-0.00444446528904442</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -2186,25 +2186,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>2.51392827451678</v>
+        <v>2.46833408038063</v>
       </c>
       <c r="F4" t="n">
-        <v>0.201082049136534</v>
+        <v>0.22714291112948</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.04507703041139</v>
+        <v>-1.03846010749416</v>
       </c>
       <c r="H4" t="n">
-        <v>0.11006605620096</v>
+        <v>0.115243977650148</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0404339904849474</v>
+        <v>0.0515939020763749</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0121145367276329</v>
+        <v>0.0132811743846279</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0187037178595124</v>
+        <v>-0.0232637853881486</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -2224,25 +2224,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>2.90225813456849</v>
+        <v>2.81382207634397</v>
       </c>
       <c r="F5" t="n">
-        <v>0.237300586670161</v>
+        <v>0.242498989040528</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.14817099226754</v>
+        <v>-1.1205857261163</v>
       </c>
       <c r="H5" t="n">
-        <v>0.105467977729247</v>
+        <v>0.101912722996449</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0563115684340025</v>
+        <v>0.0588057596856783</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0111234943262969</v>
+        <v>0.010386203108551</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.021248020735707</v>
+        <v>-0.021909225552673</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -2262,25 +2262,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>2.08586326373053</v>
+        <v>2.01849548600067</v>
       </c>
       <c r="F6" t="n">
-        <v>0.145302181619435</v>
+        <v>0.122883242611463</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.03120411829495</v>
+        <v>-1.01997434819274</v>
       </c>
       <c r="H6" t="n">
-        <v>0.074283046751274</v>
+        <v>0.0818857483036436</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0211127239833672</v>
+        <v>0.0151002913147078</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00551797103465195</v>
+        <v>0.00670527577524767</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.00869402226637252</v>
+        <v>-0.00742396882898494</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -2300,25 +2300,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>2.37960527088054</v>
+        <v>2.3420142874128</v>
       </c>
       <c r="F7" t="n">
-        <v>0.179786460979122</v>
+        <v>0.215810175558297</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.07901445539707</v>
+        <v>-1.08629849598012</v>
       </c>
       <c r="H7" t="n">
-        <v>0.10031066104669</v>
+        <v>0.13211005024603</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0323231715513972</v>
+        <v>0.0465740318745031</v>
       </c>
       <c r="J7" t="n">
-        <v>0.010062228719624</v>
+        <v>0.0174530653760086</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0162601111896603</v>
+        <v>-0.0269241863120591</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -2338,25 +2338,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>1.52166620795309</v>
+        <v>1.52982703612423</v>
       </c>
       <c r="F8" t="n">
-        <v>0.333572687350795</v>
+        <v>0.343917875306103</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.773932916603465</v>
+        <v>-0.830115526445352</v>
       </c>
       <c r="H8" t="n">
-        <v>0.135974053392742</v>
+        <v>0.186708829854108</v>
       </c>
       <c r="I8" t="n">
-        <v>0.111270737746431</v>
+        <v>0.118279504955064</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0184889431960524</v>
+        <v>0.0348601871454903</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0303399210140507</v>
+        <v>-0.0477083810907798</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -2376,25 +2376,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>2.48739055832804</v>
+        <v>2.4381676875878</v>
       </c>
       <c r="F9" t="n">
-        <v>0.423446230224185</v>
+        <v>0.484812865854487</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.07834058869686</v>
+        <v>-1.07201620635763</v>
       </c>
       <c r="H9" t="n">
-        <v>0.159202180743191</v>
+        <v>0.192364462982496</v>
       </c>
       <c r="I9" t="n">
-        <v>0.179306709891073</v>
+        <v>0.235043514898041</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0253453343533878</v>
+        <v>0.0370040866185441</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0627180539399422</v>
+        <v>-0.0878022120874772</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -2414,25 +2414,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>1.49818030642701</v>
+        <v>1.41853795862842</v>
       </c>
       <c r="F10" t="n">
-        <v>0.331222567339514</v>
+        <v>0.298670614418002</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.01418267661033</v>
+        <v>-0.997272275177952</v>
       </c>
       <c r="H10" t="n">
-        <v>0.147453826849644</v>
+        <v>0.129046366793532</v>
       </c>
       <c r="I10" t="n">
-        <v>0.109708389114979</v>
+        <v>0.089204135916827</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0217426310526049</v>
+        <v>0.0166529647826108</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0418133861145634</v>
+        <v>-0.0321888868121076</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -2452,25 +2452,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>2.01754446692552</v>
+        <v>1.91397156346093</v>
       </c>
       <c r="F11" t="n">
-        <v>0.317384281227654</v>
+        <v>0.251259573281716</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.984930211873869</v>
+        <v>-0.965044938060798</v>
       </c>
       <c r="H11" t="n">
-        <v>0.101801443691546</v>
+        <v>0.0796827302863566</v>
       </c>
       <c r="I11" t="n">
-        <v>0.100732781970394</v>
+        <v>0.0631313731657098</v>
       </c>
       <c r="J11" t="n">
-        <v>0.010363533937683</v>
+        <v>0.00634933750588825</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0284881700528722</v>
+        <v>-0.0158753027847061</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -2490,25 +2490,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>2.02696016167979</v>
+        <v>1.98537693246169</v>
       </c>
       <c r="F12" t="n">
-        <v>0.409698626967328</v>
+        <v>0.309598793339315</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.968032021305164</v>
+        <v>-0.971956116966394</v>
       </c>
       <c r="H12" t="n">
-        <v>0.161971004464799</v>
+        <v>0.12666401900976</v>
       </c>
       <c r="I12" t="n">
-        <v>0.167852964938914</v>
+        <v>0.0958514128371598</v>
       </c>
       <c r="J12" t="n">
-        <v>0.026234606287336</v>
+        <v>0.0160437737117049</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0587283707432745</v>
+        <v>-0.0289126257453649</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -2528,25 +2528,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>2.88150849650292</v>
+        <v>2.81513530583061</v>
       </c>
       <c r="F13" t="n">
-        <v>0.698101806909137</v>
+        <v>0.549529613637574</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.04537780645883</v>
+        <v>-1.03564365282378</v>
       </c>
       <c r="H13" t="n">
-        <v>0.221833270937624</v>
+        <v>0.177278779745409</v>
       </c>
       <c r="I13" t="n">
-        <v>0.487346132809803</v>
+        <v>0.301982796264662</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0492100000948854</v>
+        <v>0.0314277657480212</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.149652715148843</v>
+        <v>-0.0905067219448786</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -2566,25 +2566,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>2.24237244057441</v>
+        <v>2.20329872621066</v>
       </c>
       <c r="F14" t="n">
-        <v>0.209726581516632</v>
+        <v>0.251472192731928</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.947676440017259</v>
+        <v>-0.949589611386702</v>
       </c>
       <c r="H14" t="n">
-        <v>0.093789380646873</v>
+        <v>0.120483913853294</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0439852389946526</v>
+        <v>0.0632382637174039</v>
       </c>
       <c r="J14" t="n">
-        <v>0.00879644792212403</v>
+        <v>0.0145163734974079</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.0161834686181826</v>
+        <v>-0.0269335727041458</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -2604,25 +2604,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>2.46094374220508</v>
+        <v>2.40219799434963</v>
       </c>
       <c r="F15" t="n">
-        <v>0.264036571292589</v>
+        <v>0.234519749464493</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.01546611467525</v>
+        <v>-1.00901173307717</v>
       </c>
       <c r="H15" t="n">
-        <v>0.109562714690895</v>
+        <v>0.102287905033608</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0697153109799464</v>
+        <v>0.0549995128888884</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0120039884504384</v>
+        <v>0.0104628155161643</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.0254842257230339</v>
+        <v>-0.0211596960556413</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -2642,25 +2642,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>2.25444620048039</v>
+        <v>2.20170535405669</v>
       </c>
       <c r="F16" t="n">
-        <v>0.222341048830984</v>
+        <v>0.21892158455339</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.911033282332893</v>
+        <v>-0.902310598510134</v>
       </c>
       <c r="H16" t="n">
-        <v>0.102491288079624</v>
+        <v>0.114508545878668</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0494355419952621</v>
+        <v>0.047926660183367</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0105044641322206</v>
+        <v>0.013112207079247</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.0192375999914305</v>
+        <v>-0.0217737793079823</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -2680,25 +2680,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>0.996763855679523</v>
+        <v>0.999415283650382</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0838183464811693</v>
+        <v>0.0710460548893685</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.717453756337411</v>
+        <v>-0.710160646468684</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0396326427899414</v>
+        <v>0.0371536156696288</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00702551520683735</v>
+        <v>0.00504754191534316</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00157074637451509</v>
+        <v>0.00138039115732648</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.000964577313751146</v>
+        <v>-0.00121965787689204</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -2718,25 +2718,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>1.12639172344645</v>
+        <v>1.13237362326564</v>
       </c>
       <c r="F18" t="n">
-        <v>0.105907986747605</v>
+        <v>0.0882260712790033</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.699866140753643</v>
+        <v>-0.691559258068776</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0462881852377329</v>
+        <v>0.0375498739940975</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0112165016569309</v>
+        <v>0.00778383965332777</v>
       </c>
       <c r="J18" t="n">
-        <v>0.00214259609260268</v>
+        <v>0.0014099930369726</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.00303414204430054</v>
+        <v>-0.00251196077708807</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -2756,25 +2756,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>2.30823999869546</v>
+        <v>2.25372991308615</v>
       </c>
       <c r="F19" t="n">
-        <v>0.212100236552518</v>
+        <v>0.193599458785533</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.06317174036088</v>
+        <v>-1.05166003595957</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0883723508302685</v>
+        <v>0.0926540495239974</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0449865103456341</v>
+        <v>0.0374807504420513</v>
       </c>
       <c r="J19" t="n">
-        <v>0.00780967239126806</v>
+        <v>0.00858477289319537</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0158401672908242</v>
+        <v>-0.0159888332730207</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -2794,25 +2794,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>2.39272083727114</v>
+        <v>2.29516138426015</v>
       </c>
       <c r="F20" t="n">
-        <v>0.265967582835733</v>
+        <v>0.222364136608754</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.21578962659053</v>
+        <v>-1.17781611095422</v>
       </c>
       <c r="H20" t="n">
-        <v>0.119222995723348</v>
+        <v>0.104923760248021</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0707387551194827</v>
+        <v>0.0494458092497564</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0142141227092495</v>
+        <v>0.0110089954645841</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0289436015331549</v>
+        <v>-0.0206429316639446</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -2832,25 +2832,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>1.05257362849532</v>
+        <v>1.02869503297525</v>
       </c>
       <c r="F21" t="n">
-        <v>0.288080901041177</v>
+        <v>0.265769224642769</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.717436925236619</v>
+        <v>-0.717688599529452</v>
       </c>
       <c r="H21" t="n">
-        <v>0.124537607141585</v>
+        <v>0.103533830249769</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0829906055446962</v>
+        <v>0.0706332807672187</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0155096155925518</v>
+        <v>0.010719254006188</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0278016389585685</v>
+        <v>-0.0171998828454053</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -2870,25 +2870,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>1.89257104125165</v>
+        <v>1.85768941713106</v>
       </c>
       <c r="F22" t="n">
-        <v>0.410670123606949</v>
+        <v>0.336969112651298</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.987198951461175</v>
+        <v>-0.993295258875856</v>
       </c>
       <c r="H22" t="n">
-        <v>0.173663665314817</v>
+        <v>0.157840161947571</v>
       </c>
       <c r="I22" t="n">
-        <v>0.168649950423347</v>
+        <v>0.113548182881003</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0301590686505767</v>
+        <v>0.0249135167236354</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0611261870872031</v>
+        <v>-0.0414908144906914</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>
@@ -2960,25 +2960,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.777951348557</v>
+        <v>-1.72519678835276</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0825379900743899</v>
+        <v>0.0869111420140341</v>
       </c>
       <c r="G2" t="n">
-        <v>1.97995936195322</v>
+        <v>1.99546287416998</v>
       </c>
       <c r="H2" t="n">
-        <v>0.170398111443839</v>
+        <v>0.204557243415721</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00681251980552008</v>
+        <v>0.00755354660618361</v>
       </c>
       <c r="J2" t="n">
-        <v>0.029035516383627</v>
+        <v>0.0418436658338387</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00435767837685548</v>
+        <v>0.00949575258569563</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -2998,25 +2998,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.99340653773269</v>
+        <v>-1.93060133863177</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0976327313995331</v>
+        <v>0.102811464864021</v>
       </c>
       <c r="G3" t="n">
-        <v>1.71303918195678</v>
+        <v>1.71540910960479</v>
       </c>
       <c r="H3" t="n">
-        <v>0.134327318012769</v>
+        <v>0.128615701649951</v>
       </c>
       <c r="I3" t="n">
-        <v>0.00953215024053337</v>
+        <v>0.0105701973074859</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0180438283645037</v>
+        <v>0.0165419987109093</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00295229503785695</v>
+        <v>0.00506328286632033</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -3036,25 +3036,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.36474220234867</v>
+        <v>-2.3370003112681</v>
       </c>
       <c r="F4" t="n">
-        <v>0.137854567634377</v>
+        <v>0.129544185691206</v>
       </c>
       <c r="G4" t="n">
-        <v>1.75745630420685</v>
+        <v>1.73953940198937</v>
       </c>
       <c r="H4" t="n">
-        <v>0.196502431741154</v>
+        <v>0.208695357802345</v>
       </c>
       <c r="I4" t="n">
-        <v>0.019003881817661</v>
+        <v>0.0167816960463977</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0386132056801868</v>
+        <v>0.0435537523682489</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0156685419146</v>
+        <v>0.0130353650991837</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -3074,25 +3074,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.5105798322056</v>
+        <v>-2.48934273642372</v>
       </c>
       <c r="F5" t="n">
-        <v>0.127186380028304</v>
+        <v>0.116141918019508</v>
       </c>
       <c r="G5" t="n">
-        <v>1.92005824140022</v>
+        <v>1.86641737773398</v>
       </c>
       <c r="H5" t="n">
-        <v>0.188394857236494</v>
+        <v>0.18441970056748</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0161763752647042</v>
+        <v>0.0134889451212501</v>
       </c>
       <c r="J5" t="n">
-        <v>0.035492622233159</v>
+        <v>0.034010625957399</v>
       </c>
       <c r="K5" t="n">
-        <v>0.00921423442182592</v>
+        <v>0.00574248268227631</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -3112,25 +3112,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.98994626729784</v>
+        <v>-1.94481970743779</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0920141316934637</v>
+        <v>0.105783665680401</v>
       </c>
       <c r="G6" t="n">
-        <v>1.79498497634401</v>
+        <v>1.78244840612281</v>
       </c>
       <c r="H6" t="n">
-        <v>0.128896134524951</v>
+        <v>0.145920306625554</v>
       </c>
       <c r="I6" t="n">
-        <v>0.00846660043130209</v>
+        <v>0.0111901839247827</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0166142134954742</v>
+        <v>0.0212927358856957</v>
       </c>
       <c r="K6" t="n">
-        <v>0.00275811421770208</v>
+        <v>0.00854226654679157</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -3150,25 +3150,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.12776853505119</v>
+        <v>-2.08438385665272</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0802505639146212</v>
+        <v>0.0833283834066869</v>
       </c>
       <c r="G7" t="n">
-        <v>1.98880947565455</v>
+        <v>2.00821523370502</v>
       </c>
       <c r="H7" t="n">
-        <v>0.20637586173419</v>
+        <v>0.264693199286976</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0064401530086147</v>
+        <v>0.00694361948117181</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0425909963065297</v>
+        <v>0.0700624897487748</v>
       </c>
       <c r="K7" t="n">
-        <v>0.00833438912926197</v>
+        <v>0.01381622202849</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -3188,25 +3188,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.9482535140164</v>
+        <v>-1.83920081528535</v>
       </c>
       <c r="F8" t="n">
-        <v>0.320334372530899</v>
+        <v>0.283458625754857</v>
       </c>
       <c r="G8" t="n">
-        <v>1.32235172671317</v>
+        <v>1.43323566724509</v>
       </c>
       <c r="H8" t="n">
-        <v>0.262812832553977</v>
+        <v>0.380173870798206</v>
       </c>
       <c r="I8" t="n">
-        <v>0.102614110224765</v>
+        <v>0.0803487925148324</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0690705849550449</v>
+        <v>0.144532172037691</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0117860403329519</v>
+        <v>0.0219698548481498</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -3226,25 +3226,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.3202820840382</v>
+        <v>-2.28588536418224</v>
       </c>
       <c r="F9" t="n">
-        <v>0.12396398295321</v>
+        <v>0.118148159030896</v>
       </c>
       <c r="G9" t="n">
-        <v>2.01411001829335</v>
+        <v>1.97834259892908</v>
       </c>
       <c r="H9" t="n">
-        <v>0.341808204640746</v>
+        <v>0.38226490490551</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0153670690696236</v>
+        <v>0.01395898748239</v>
       </c>
       <c r="J9" t="n">
-        <v>0.11683284875973</v>
+        <v>0.146126457522419</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.00454031818455012</v>
+        <v>-0.00159880999586965</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -3264,25 +3264,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.51780137431937</v>
+        <v>-1.45210266844635</v>
       </c>
       <c r="F10" t="n">
-        <v>0.174083053785454</v>
+        <v>0.163509255779092</v>
       </c>
       <c r="G10" t="n">
-        <v>1.80764729238051</v>
+        <v>1.76506582427408</v>
       </c>
       <c r="H10" t="n">
-        <v>0.276044299109395</v>
+        <v>0.238246846292879</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0303049096152694</v>
+        <v>0.0267352767254325</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0762004550707972</v>
+        <v>0.0567615597685027</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0131148317432069</v>
+        <v>-0.0101279729218984</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -3302,25 +3302,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.1068711084345</v>
+        <v>-2.0339517655342</v>
       </c>
       <c r="F11" t="n">
-        <v>0.179161935426299</v>
+        <v>0.179930231478184</v>
       </c>
       <c r="G11" t="n">
-        <v>1.70033738522035</v>
+        <v>1.64617655510194</v>
       </c>
       <c r="H11" t="n">
-        <v>0.208460945649327</v>
+        <v>0.157352972748654</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0320989991056973</v>
+        <v>0.0323748881997928</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0434559658610115</v>
+        <v>0.0247599580328386</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.016561795590602</v>
+        <v>-0.00937185231836174</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -3340,25 +3340,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.12000443797963</v>
+        <v>-2.07102831617382</v>
       </c>
       <c r="F12" t="n">
-        <v>0.195730672493874</v>
+        <v>0.21136996067186</v>
       </c>
       <c r="G12" t="n">
-        <v>1.68474374822919</v>
+        <v>1.68163101716978</v>
       </c>
       <c r="H12" t="n">
-        <v>0.298690654707669</v>
+        <v>0.224759741543284</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0383104961549042</v>
+        <v>0.0446772602744237</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0892161072096957</v>
+        <v>0.0505169414186039</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.00718671917003027</v>
+        <v>0.00891023701979488</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -3378,25 +3378,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>-2.79988513554914</v>
+        <v>-2.76933170304976</v>
       </c>
       <c r="F13" t="n">
-        <v>0.164643636088581</v>
+        <v>0.177956593636583</v>
       </c>
       <c r="G13" t="n">
-        <v>1.91886556853772</v>
+        <v>1.91020861268176</v>
       </c>
       <c r="H13" t="n">
-        <v>0.416384465763807</v>
+        <v>0.371607190811063</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0271075269044691</v>
+        <v>0.0316685492187359</v>
       </c>
       <c r="J13" t="n">
-        <v>0.173376023329411</v>
+        <v>0.13809190426249</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0160310530185101</v>
+        <v>-0.0048304199862856</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -3416,25 +3416,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>-2.33221811018217</v>
+        <v>-2.29189352078826</v>
       </c>
       <c r="F14" t="n">
-        <v>0.13146167929006</v>
+        <v>0.134661724775328</v>
       </c>
       <c r="G14" t="n">
-        <v>1.63784568118737</v>
+        <v>1.63959728057625</v>
       </c>
       <c r="H14" t="n">
-        <v>0.182955046239077</v>
+        <v>0.243901739439504</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0172821731217626</v>
+        <v>0.0181337801194661</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0334725489443429</v>
+        <v>0.0594880585016157</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00660130343739672</v>
+        <v>0.0106255584561674</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -3454,25 +3454,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.40113898532518</v>
+        <v>-2.35918673923445</v>
       </c>
       <c r="F15" t="n">
-        <v>0.122189329723341</v>
+        <v>0.116437894083279</v>
       </c>
       <c r="G15" t="n">
-        <v>1.77239131003522</v>
+        <v>1.75657302549737</v>
       </c>
       <c r="H15" t="n">
-        <v>0.201440275309019</v>
+        <v>0.210949146448444</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0149302322982393</v>
+        <v>0.013557783178549</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0405781845165733</v>
+        <v>0.0444995423873269</v>
       </c>
       <c r="K15" t="n">
-        <v>0.00513875423267739</v>
+        <v>0.00663085164219347</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -3492,25 +3492,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.4143783123601</v>
+        <v>-2.38452510033337</v>
       </c>
       <c r="F16" t="n">
-        <v>0.137942025672175</v>
+        <v>0.149022890586942</v>
       </c>
       <c r="G16" t="n">
-        <v>1.60198656443551</v>
+        <v>1.58591775413186</v>
       </c>
       <c r="H16" t="n">
-        <v>0.208027541326574</v>
+        <v>0.246475210808504</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0190280024465431</v>
+        <v>0.0222078219188878</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0432754579503796</v>
+        <v>0.0607500295430965</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0126785340110562</v>
+        <v>0.0211604529847967</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -3530,25 +3530,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.35404457784318</v>
+        <v>-1.37351061111828</v>
       </c>
       <c r="F17" t="n">
-        <v>0.128536016420039</v>
+        <v>0.0975451183537697</v>
       </c>
       <c r="G17" t="n">
-        <v>1.19415857248779</v>
+        <v>1.17954533219363</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0721988778408155</v>
+        <v>0.064612489657263</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0165215075171325</v>
+        <v>0.00951505011465093</v>
       </c>
       <c r="J17" t="n">
-        <v>0.005212677961473</v>
+        <v>0.00417477381970992</v>
       </c>
       <c r="K17" t="n">
-        <v>0.00281371419096406</v>
+        <v>0.00140889801365611</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -3568,25 +3568,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.61323348320391</v>
+        <v>-1.64016821659955</v>
       </c>
       <c r="F18" t="n">
-        <v>0.121792974479335</v>
+        <v>0.0855002121713666</v>
       </c>
       <c r="G18" t="n">
-        <v>1.20063498888004</v>
+        <v>1.1820943127845</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0808011520191903</v>
+        <v>0.0656643713394952</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0148335286325239</v>
+        <v>0.0073102862813487</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0065288261676283</v>
+        <v>0.00431180966341111</v>
       </c>
       <c r="K18" t="n">
-        <v>0.00119713614630879</v>
+        <v>-0.000502977650851661</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -3606,25 +3606,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.16821355133828</v>
+        <v>-2.14081736529117</v>
       </c>
       <c r="F19" t="n">
-        <v>0.108395064222108</v>
+        <v>0.0953969328983439</v>
       </c>
       <c r="G19" t="n">
-        <v>1.82811151936182</v>
+        <v>1.80317848000473</v>
       </c>
       <c r="H19" t="n">
-        <v>0.165729340740227</v>
+        <v>0.177904693938904</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0117494899477149</v>
+        <v>0.00910057480641112</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0274662143821902</v>
+        <v>0.0316500801254951</v>
       </c>
       <c r="K19" t="n">
-        <v>0.000984596875272105</v>
+        <v>0.00299024922680052</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -3644,25 +3644,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.99064811632014</v>
+        <v>-1.97028949193194</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0821751582283421</v>
+        <v>0.0801902518794047</v>
       </c>
       <c r="G20" t="n">
-        <v>2.20498659844789</v>
+        <v>2.12084194642728</v>
       </c>
       <c r="H20" t="n">
-        <v>0.237363083214124</v>
+        <v>0.213035641702335</v>
       </c>
       <c r="I20" t="n">
-        <v>0.00675275662985306</v>
+        <v>0.00643047649648237</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0563412332729153</v>
+        <v>0.0453841846355257</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.00363605265518199</v>
+        <v>-0.00257506918792403</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -3682,25 +3682,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.50596150897498</v>
+        <v>-1.46716693033476</v>
       </c>
       <c r="F21" t="n">
-        <v>0.249752256684582</v>
+        <v>0.287705749115125</v>
       </c>
       <c r="G21" t="n">
-        <v>1.26653750603206</v>
+        <v>1.26059972867232</v>
       </c>
       <c r="H21" t="n">
-        <v>0.216449955109887</v>
+        <v>0.170502953872554</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0623761897190414</v>
+        <v>0.0827745980738954</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0468505830670721</v>
+        <v>0.0290712572792663</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.007029593649587</v>
+        <v>0.0044798074636298</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -3720,25 +3720,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>-1.94606176905585</v>
+        <v>-1.89524984654235</v>
       </c>
       <c r="F22" t="n">
-        <v>0.208222229400172</v>
+        <v>0.220566185666429</v>
       </c>
       <c r="G22" t="n">
-        <v>1.74164222910467</v>
+        <v>1.75319588941478</v>
       </c>
       <c r="H22" t="n">
-        <v>0.353357713227375</v>
+        <v>0.328357094076466</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0433564968163777</v>
+        <v>0.0486494422594377</v>
       </c>
       <c r="J22" t="n">
-        <v>0.12486167349728</v>
+        <v>0.107818381230341</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.00783054883103203</v>
+        <v>0.00702714895855935</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>
@@ -3810,25 +3810,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.08140174659871</v>
+        <v>-2.01765690253255</v>
       </c>
       <c r="F2" t="n">
-        <v>0.101464536652</v>
+        <v>0.103447449067094</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.0180406304756775</v>
+        <v>-0.0190740131440861</v>
       </c>
       <c r="H2" t="n">
-        <v>0.012319060510442</v>
+        <v>0.0138713780231997</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0102950521980051</v>
+        <v>0.0107013747184891</v>
       </c>
       <c r="J2" t="n">
-        <v>0.000151759251859932</v>
+        <v>0.000192415128262507</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.000601428257233394</v>
+        <v>-0.00050452431854454</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -3848,25 +3848,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.3636120790641</v>
+        <v>-2.29339372378354</v>
       </c>
       <c r="F3" t="n">
-        <v>0.126087808930259</v>
+        <v>0.132301106530333</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0125577421591243</v>
+        <v>-0.013784129933345</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00856252069692879</v>
+        <v>0.00673971626319614</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0158981355608334</v>
+        <v>0.0175035827891505</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0000733167606853339</v>
+        <v>0.0000454237753083905</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.000677055669639301</v>
+        <v>-0.00054132285507576</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -3886,25 +3886,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.70193626478097</v>
+        <v>-2.66618220861419</v>
       </c>
       <c r="F4" t="n">
-        <v>0.156444834207228</v>
+        <v>0.144808633201942</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0190879804587354</v>
+        <v>-0.0198690908444268</v>
       </c>
       <c r="H4" t="n">
-        <v>0.019550634465166</v>
+        <v>0.0191775399753587</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0244749861501269</v>
+        <v>0.0209695402498145</v>
       </c>
       <c r="J4" t="n">
-        <v>0.000382227307990537</v>
+        <v>0.00036777803950648</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.00172192507099017</v>
+        <v>-0.00167073607669963</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -3924,25 +3924,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>-3.06419331756653</v>
+        <v>-3.00530460641232</v>
       </c>
       <c r="F5" t="n">
-        <v>0.185570645347155</v>
+        <v>0.175142582567864</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0121285462350868</v>
+        <v>0.00745643115831869</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0163362747356503</v>
+        <v>0.0142202203186205</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0344364644145594</v>
+        <v>0.0306749242285411</v>
       </c>
       <c r="J5" t="n">
-        <v>0.000266873872238646</v>
+        <v>0.000202214665910108</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.00195349293902929</v>
+        <v>-0.00183131118844048</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -3962,25 +3962,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.23135235698007</v>
+        <v>-2.17249190145231</v>
       </c>
       <c r="F6" t="n">
-        <v>0.101177196866545</v>
+        <v>0.111546443989113</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0235283723645498</v>
+        <v>-0.0268888286602143</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00996964691214282</v>
+        <v>0.00923898580002034</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0102368251657716</v>
+        <v>0.0124426091666163</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0000993938595527989</v>
+        <v>0.0000853588586129775</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.000595977887148311</v>
+        <v>-0.000441079631820998</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -4000,25 +4000,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.30353901599517</v>
+        <v>-2.25929198323504</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0849990247310865</v>
+        <v>0.08253900642319</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0295289955002821</v>
+        <v>-0.0299328683024798</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00740228834920616</v>
+        <v>0.0095122801950541</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00722483420523586</v>
+        <v>0.0068126875813274</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0000547938728047933</v>
+        <v>0.0000904834745092185</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.000207469315286281</v>
+        <v>-0.000146717072827743</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -4038,25 +4038,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.2271083115886</v>
+        <v>-2.15271197631863</v>
       </c>
       <c r="F8" t="n">
-        <v>0.34245155985288</v>
+        <v>0.295240845282059</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0377432470081011</v>
+        <v>-0.0312207305439134</v>
       </c>
       <c r="H8" t="n">
-        <v>0.030834685943283</v>
+        <v>0.0287361000618847</v>
       </c>
       <c r="I8" t="n">
-        <v>0.117273070845671</v>
+        <v>0.0871671567228649</v>
       </c>
       <c r="J8" t="n">
-        <v>0.000950777857220891</v>
+        <v>0.000825763446766651</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.00652736343257616</v>
+        <v>-0.00352109315215479</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -4076,25 +4076,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.65972894717063</v>
+        <v>-2.65027185824501</v>
       </c>
       <c r="F9" t="n">
-        <v>0.189263107546043</v>
+        <v>0.225090686544683</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.00246882176944569</v>
+        <v>0.00000447698641238702</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0180428086912718</v>
+        <v>0.0270325818460841</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0358205238779849</v>
+        <v>0.0506658171691567</v>
       </c>
       <c r="J9" t="n">
-        <v>0.000325542945469833</v>
+        <v>0.000730760481265237</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.00230345389205733</v>
+        <v>-0.00415997704233024</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -4114,25 +4114,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.02381715538323</v>
+        <v>-1.9226526959951</v>
       </c>
       <c r="F10" t="n">
-        <v>0.255778640267797</v>
+        <v>0.2434248993688</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0255597996111659</v>
+        <v>0.0148059705014051</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0404981984260776</v>
+        <v>0.0463504303092982</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0654227128172429</v>
+        <v>0.0592556816327103</v>
       </c>
       <c r="J10" t="n">
-        <v>0.00164010407575795</v>
+        <v>0.00214836238985711</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.00711036413780034</v>
+        <v>-0.00869296177512084</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -4152,25 +4152,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.67178985962201</v>
+        <v>-2.58753790062641</v>
       </c>
       <c r="F11" t="n">
-        <v>0.230673825428547</v>
+        <v>0.210820747593303</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0177692748011179</v>
+        <v>0.0146205057425297</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0167409973495209</v>
+        <v>0.0191134696191717</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0532104137378396</v>
+        <v>0.0444453876157992</v>
       </c>
       <c r="J11" t="n">
-        <v>0.000280260992256664</v>
+        <v>0.000365324720882999</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.00252369250313782</v>
+        <v>-0.00225609370786197</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -4190,25 +4190,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.61749017114501</v>
+        <v>-2.54933555186575</v>
       </c>
       <c r="F12" t="n">
-        <v>0.28894923044443</v>
+        <v>0.249008871886208</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0123792653404658</v>
+        <v>0.0102466828139336</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0306305115929061</v>
+        <v>0.0195441948683702</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0834916577744283</v>
+        <v>0.0620054182780418</v>
       </c>
       <c r="J12" t="n">
-        <v>0.000938228240443155</v>
+        <v>0.000381975553052829</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0063487416996439</v>
+        <v>-0.00214364487714964</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -4228,25 +4228,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>-3.46876419652843</v>
+        <v>-3.42672233937081</v>
       </c>
       <c r="F13" t="n">
-        <v>0.299780689171852</v>
+        <v>0.243199656921414</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0242905260330743</v>
+        <v>0.0243636821714332</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0184675218673625</v>
+        <v>0.0122956675768103</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0898684616003503</v>
+        <v>0.0591460731266934</v>
       </c>
       <c r="J13" t="n">
-        <v>0.000341049363921511</v>
+        <v>0.000151183441159423</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0041447436937204</v>
+        <v>-0.00126953734763064</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -4266,25 +4266,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>-2.53774537520061</v>
+        <v>-2.49902757553759</v>
       </c>
       <c r="F14" t="n">
-        <v>0.141652278771847</v>
+        <v>0.151796300191924</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0256502815535124</v>
+        <v>-0.0260432363531547</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0115962452167281</v>
+        <v>0.012122266923568</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0200653680812571</v>
+        <v>0.0230421167519567</v>
       </c>
       <c r="J14" t="n">
-        <v>0.00013447290312649</v>
+        <v>0.000146949355366231</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.000884315954813601</v>
+        <v>-0.000973927502218067</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -4304,25 +4304,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.64863060347219</v>
+        <v>-2.60453622180521</v>
       </c>
       <c r="F15" t="n">
-        <v>0.140374272993617</v>
+        <v>0.140775675694235</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.0168393407736236</v>
+        <v>-0.0179874448132232</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0119133252065979</v>
+        <v>0.00981579720341566</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0197049365184865</v>
+        <v>0.0198177908671686</v>
       </c>
       <c r="J15" t="n">
-        <v>0.000141927317478162</v>
+        <v>0.0000963498747385826</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.000937601013814208</v>
+        <v>-0.000793480139508984</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -4342,25 +4342,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.51123869942539</v>
+        <v>-2.47257403697872</v>
       </c>
       <c r="F16" t="n">
-        <v>0.121563063431743</v>
+        <v>0.1067374594493</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0369299932610897</v>
+        <v>-0.0386901786342452</v>
       </c>
       <c r="H16" t="n">
-        <v>0.010499509130997</v>
+        <v>0.00949365882628895</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01477757839091</v>
+        <v>0.011392885249691</v>
       </c>
       <c r="J16" t="n">
-        <v>0.000110239691991889</v>
+        <v>0.000090129557909974</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.000462489919387872</v>
+        <v>-0.0000163124782557576</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -4380,25 +4380,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.56961926885366</v>
+        <v>-1.59135908631409</v>
       </c>
       <c r="F17" t="n">
-        <v>0.130599670361597</v>
+        <v>0.0932982144745055</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.0906814699721602</v>
+        <v>-0.0889611671755879</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0202486490166893</v>
+        <v>0.0166836023152949</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0170562738985578</v>
+        <v>0.00870455682413083</v>
       </c>
       <c r="J17" t="n">
-        <v>0.000410007787001074</v>
+        <v>0.000278342586214914</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.00191837604648169</v>
+        <v>-0.00105036762195595</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -4418,25 +4418,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.84249044736258</v>
+        <v>-1.86178907503081</v>
       </c>
       <c r="F18" t="n">
-        <v>0.127874783169237</v>
+        <v>0.0914459151885326</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0639210532659732</v>
+        <v>-0.0646415225040878</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0168349599084398</v>
+        <v>0.0128324640774315</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0163519601705793</v>
+        <v>0.0083623554046683</v>
       </c>
       <c r="J18" t="n">
-        <v>0.000283415875118776</v>
+        <v>0.000164672134298569</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.00153860905264522</v>
+        <v>-0.00089930462489449</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -4456,25 +4456,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.56149356438312</v>
+        <v>-2.53105087692342</v>
       </c>
       <c r="F19" t="n">
-        <v>0.14962558407627</v>
+        <v>0.130124689890718</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.00129002285038163</v>
+        <v>-0.00238000384600223</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0138376768307981</v>
+        <v>0.0140000910362655</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0223878154101648</v>
+        <v>0.0169324349191557</v>
       </c>
       <c r="J19" t="n">
-        <v>0.000191481300073606</v>
+        <v>0.000196002549023721</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.00137946959787476</v>
+        <v>-0.00125060303915194</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -4494,25 +4494,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.34740021745688</v>
+        <v>-2.29936955689108</v>
       </c>
       <c r="F20" t="n">
-        <v>0.126118366223994</v>
+        <v>0.105835268383319</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00794657992825708</v>
+        <v>0.00178324955458855</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0201871014722952</v>
+        <v>0.0170697952170677</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0159058422990094</v>
+        <v>0.0112011040337692</v>
       </c>
       <c r="J20" t="n">
-        <v>0.000407519065852742</v>
+        <v>0.000291377908752626</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0017874632243433</v>
+        <v>-0.0010767979983474</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -4532,25 +4532,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.8334625702322</v>
+        <v>-1.77351822022407</v>
       </c>
       <c r="F21" t="n">
-        <v>0.270318049401206</v>
+        <v>0.320554106187069</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.0444484446995318</v>
+        <v>-0.0531899742245637</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0368542173565487</v>
+        <v>0.0449845807907303</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0730718478320728</v>
+        <v>0.10275493499339</v>
       </c>
       <c r="J21" t="n">
-        <v>0.00135823333696374</v>
+        <v>0.00202361250891774</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.00680553207578169</v>
+        <v>-0.0106890316796556</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -4570,25 +4570,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>-2.50741289770736</v>
+        <v>-2.39640552258822</v>
       </c>
       <c r="F22" t="n">
-        <v>0.318208850704761</v>
+        <v>0.274374733260961</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0248428547262417</v>
+        <v>0.0140410826723287</v>
       </c>
       <c r="H22" t="n">
-        <v>0.047688533074933</v>
+        <v>0.0322726576179848</v>
       </c>
       <c r="I22" t="n">
-        <v>0.101256872666845</v>
+        <v>0.0752814942520235</v>
       </c>
       <c r="J22" t="n">
-        <v>0.00227419618683898</v>
+        <v>0.00104152442972767</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0101235506567224</v>
+        <v>-0.00475935260339732</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
code and example output for HR and survival plots
</commit_message>
<xml_diff>
--- a/Data/bugsdata/parametric survival bugs data.xlsx
+++ b/Data/bugsdata/parametric survival bugs data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -470,12 +470,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1147,12 +1147,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1201,12 +1201,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1260,25 +1260,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.33006830871177</v>
+        <v>-2.39500202175584</v>
       </c>
       <c r="F2" t="n">
-        <v>0.10533870155035</v>
+        <v>0.10812372759168</v>
       </c>
       <c r="G2" t="n">
-        <v>0.105924771630349</v>
+        <v>0.103772517733394</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0881247958125287</v>
+        <v>0.0769739957034721</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0110962420443137</v>
+        <v>0.0116907404683198</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00776597963699988</v>
+        <v>0.00592499601455814</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.00350576567788289</v>
+        <v>-0.00402251489432989</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -1298,25 +1298,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.49972872840229</v>
+        <v>-2.57824772385901</v>
       </c>
       <c r="F3" t="n">
-        <v>0.122057447093382</v>
+        <v>0.125256517287666</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0391414385130606</v>
+        <v>0.0468565894924138</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0517908396172799</v>
+        <v>0.05928365352867</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0148980203909537</v>
+        <v>0.0156891951230354</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00268229106826281</v>
+        <v>0.00351455157570738</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.00257155016007909</v>
+        <v>-0.00425682222495584</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -1336,25 +1336,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-3.09126802584416</v>
+        <v>-3.13810935882744</v>
       </c>
       <c r="F4" t="n">
-        <v>0.175312283413101</v>
+        <v>0.188580141371055</v>
       </c>
       <c r="G4" t="n">
-        <v>0.143473106550909</v>
+        <v>0.150618291702876</v>
       </c>
       <c r="H4" t="n">
-        <v>0.117818399725227</v>
+        <v>0.122038959982672</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0307343967155154</v>
+        <v>0.0355624697195271</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0138811753138134</v>
+        <v>0.0148935077536523</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0141763938303875</v>
+        <v>-0.0152701894491901</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -1374,25 +1374,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>-3.48734749630726</v>
+        <v>-3.58822680878078</v>
       </c>
       <c r="F5" t="n">
-        <v>0.242367660737922</v>
+        <v>0.250481693413968</v>
       </c>
       <c r="G5" t="n">
-        <v>0.282416396265322</v>
+        <v>0.327498708634429</v>
       </c>
       <c r="H5" t="n">
-        <v>0.11231437447069</v>
+        <v>0.118770393218704</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0587420829715727</v>
+        <v>0.0627410787355289</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0126145187127423</v>
+        <v>0.0141064063053257</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0229317679615367</v>
+        <v>-0.0232967607253938</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -1412,25 +1412,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.41945335488241</v>
+        <v>-2.48739851639861</v>
       </c>
       <c r="F6" t="n">
-        <v>0.107605083706125</v>
+        <v>0.119237197740365</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0399294119806398</v>
+        <v>-0.0173439251044164</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0802228258285359</v>
+        <v>0.0858621209145547</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0115788540394022</v>
+        <v>0.0142175093249749</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00643570178391561</v>
+        <v>0.00737230380794561</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.00318512887970389</v>
+        <v>-0.00675677729281162</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -1450,25 +1450,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.56891849151363</v>
+        <v>-2.61351770303824</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0953207574839895</v>
+        <v>0.0912646059721666</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0434775808987697</v>
+        <v>-0.0447916602245716</v>
       </c>
       <c r="H7" t="n">
-        <v>0.101936547928577</v>
+        <v>0.0750187544228287</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00908604680732155</v>
+        <v>0.00832922830325483</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0103910598035951</v>
+        <v>0.00562781351515267</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.00562530671538125</v>
+        <v>-0.00329069460677465</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -1488,25 +1488,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.28927585322432</v>
+        <v>-2.35992376256339</v>
       </c>
       <c r="F8" t="n">
-        <v>0.263546347264198</v>
+        <v>0.309719915328088</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.107253607990594</v>
+        <v>-0.153144231507661</v>
       </c>
       <c r="H8" t="n">
-        <v>0.169984735668374</v>
+        <v>0.150161873039823</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0694566771563014</v>
+        <v>0.0959264259508379</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0288948103602471</v>
+        <v>0.0225485881148278</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0143544642403251</v>
+        <v>-0.0218092681903502</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -1526,25 +1526,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.97605246674702</v>
+        <v>-3.00978071494291</v>
       </c>
       <c r="F9" t="n">
-        <v>0.323540867216825</v>
+        <v>0.294620451678279</v>
       </c>
       <c r="G9" t="n">
-        <v>0.137278719565766</v>
+        <v>0.138978900167005</v>
       </c>
       <c r="H9" t="n">
-        <v>0.216077907045135</v>
+        <v>0.170187449721332</v>
       </c>
       <c r="I9" t="n">
-        <v>0.104678692759415</v>
+        <v>0.086801210547113</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0466896619130061</v>
+        <v>0.0289637680426511</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0591706299533721</v>
+        <v>-0.0421769037283446</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -1564,25 +1564,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.0472551672577</v>
+        <v>-2.14218267845162</v>
       </c>
       <c r="F10" t="n">
-        <v>0.261938085818681</v>
+        <v>0.273912315481934</v>
       </c>
       <c r="G10" t="n">
-        <v>0.155430830791449</v>
+        <v>0.1969390943671</v>
       </c>
       <c r="H10" t="n">
-        <v>0.172266877897778</v>
+        <v>0.161633137077179</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0686115608023547</v>
+        <v>0.0750279565726748</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0296758772206481</v>
+        <v>0.0261252710014103</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0339121655313017</v>
+        <v>-0.0311812098035073</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -1602,25 +1602,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.6879308622404</v>
+        <v>-2.82367267232602</v>
       </c>
       <c r="F11" t="n">
-        <v>0.254893879407089</v>
+        <v>0.324682196980101</v>
       </c>
       <c r="G11" t="n">
-        <v>0.130167622053188</v>
+        <v>0.175621856814685</v>
       </c>
       <c r="H11" t="n">
-        <v>0.11158061989941</v>
+        <v>0.13578283802204</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0649708897591956</v>
+        <v>0.105418529035825</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0124502347371367</v>
+        <v>0.0184369791013194</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0206858569923194</v>
+        <v>-0.0377651881515243</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -1640,25 +1640,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.76488446758512</v>
+        <v>-2.85084742220134</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2959383108534</v>
+        <v>0.373118632041817</v>
       </c>
       <c r="G12" t="n">
-        <v>0.174964827340232</v>
+        <v>0.191139707450786</v>
       </c>
       <c r="H12" t="n">
-        <v>0.114840037842542</v>
+        <v>0.184639301058125</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0875794838307637</v>
+        <v>0.139217513576757</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0131882342916765</v>
+        <v>0.034091671495233</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0198566769345156</v>
+        <v>-0.0563951175806997</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -1678,25 +1678,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>-3.92419203737332</v>
+        <v>-4.00779465950803</v>
       </c>
       <c r="F13" t="n">
-        <v>0.494772230509085</v>
+        <v>0.628093159789506</v>
       </c>
       <c r="G13" t="n">
-        <v>0.360426783558681</v>
+        <v>0.375222007563247</v>
       </c>
       <c r="H13" t="n">
-        <v>0.187127507302931</v>
+        <v>0.244402793342619</v>
       </c>
       <c r="I13" t="n">
-        <v>0.244799560082935</v>
+        <v>0.394501017374366</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0350167039894086</v>
+        <v>0.059732725393675</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0810677652745029</v>
+        <v>-0.14457190032534</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -1716,25 +1716,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>-2.79738339481437</v>
+        <v>-2.84402157787172</v>
       </c>
       <c r="F14" t="n">
-        <v>0.171698196289065</v>
+        <v>0.166400404319523</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0139801110920569</v>
+        <v>-0.0114217344621236</v>
       </c>
       <c r="H14" t="n">
-        <v>0.105889677952872</v>
+        <v>0.0918101730715185</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0294802706089184</v>
+        <v>0.0276890945577009</v>
       </c>
       <c r="J14" t="n">
-        <v>0.011212623896963</v>
+        <v>0.00842910787942218</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.0116199924086907</v>
+        <v>-0.00936032305604423</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -1754,25 +1754,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.95410791709162</v>
+        <v>-3.01920941114309</v>
       </c>
       <c r="F15" t="n">
-        <v>0.173133254677496</v>
+        <v>0.1957543823296</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0556593266224006</v>
+        <v>0.0688710722139505</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0926145582214106</v>
+        <v>0.106918285891009</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0299751238752225</v>
+        <v>0.0383197782012431</v>
       </c>
       <c r="J15" t="n">
-        <v>0.00857745639454706</v>
+        <v>0.0114315198578715</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.0112536040524681</v>
+        <v>-0.0153403431417579</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -1792,25 +1792,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.79756053367509</v>
+        <v>-2.8473150791631</v>
       </c>
       <c r="F16" t="n">
-        <v>0.119642980975563</v>
+        <v>0.144695958439284</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0884476008590871</v>
+        <v>-0.0750160783595377</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0838583312620675</v>
+        <v>0.0858304841970044</v>
       </c>
       <c r="I16" t="n">
-        <v>0.014314442896719</v>
+        <v>0.0209369203886629</v>
       </c>
       <c r="J16" t="n">
-        <v>0.00703221972205866</v>
+        <v>0.00736687201749222</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.00234476540435095</v>
+        <v>-0.00586329307363494</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -1830,25 +1830,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.8496768167544</v>
+        <v>-1.83658401006587</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0713815590614557</v>
+        <v>0.0953889499198419</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.201232123211273</v>
+        <v>-0.197722113791001</v>
       </c>
       <c r="H17" t="n">
-        <v>0.036854147082554</v>
+        <v>0.0419833442232253</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00509532697404409</v>
+        <v>0.00909905176681011</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00135822815718253</v>
+        <v>0.00176260119216583</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.000288346995536712</v>
+        <v>-0.000608601100755223</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -1868,25 +1868,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>-2.04690973252514</v>
+        <v>-2.02920667547382</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0737316968516354</v>
+        <v>0.101386015116349</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.171946395700535</v>
+        <v>-0.165252558924571</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0388523711236188</v>
+        <v>0.04858091302945</v>
       </c>
       <c r="I18" t="n">
-        <v>0.00543636312062147</v>
+        <v>0.0102791240611726</v>
       </c>
       <c r="J18" t="n">
-        <v>0.00150950674192741</v>
+        <v>0.00236010511077498</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.00158773213442984</v>
+        <v>-0.0018486256997203</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -1906,25 +1906,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.83545108599723</v>
+        <v>-2.88701180933812</v>
       </c>
       <c r="F19" t="n">
-        <v>0.159160874987795</v>
+        <v>0.187647325679811</v>
       </c>
       <c r="G19" t="n">
-        <v>0.145673114301433</v>
+        <v>0.161475571525528</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0977476357725525</v>
+        <v>0.0969665892615014</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0253321841268806</v>
+        <v>0.035211518834785</v>
       </c>
       <c r="J19" t="n">
-        <v>0.00955460029912358</v>
+        <v>0.00940251943300871</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0120621687812353</v>
+        <v>-0.0137431723158013</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -1944,25 +1944,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.72194870874295</v>
+        <v>-2.80076969518453</v>
       </c>
       <c r="F20" t="n">
-        <v>0.163891712200428</v>
+        <v>0.199420834984694</v>
       </c>
       <c r="G20" t="n">
-        <v>0.255836150826446</v>
+        <v>0.300144465918335</v>
       </c>
       <c r="H20" t="n">
-        <v>0.118697956862633</v>
+        <v>0.135723151780683</v>
       </c>
       <c r="I20" t="n">
-        <v>0.026860493327988</v>
+        <v>0.0397686694259927</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0140892049633635</v>
+        <v>0.0184207739292822</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0149839404293542</v>
+        <v>-0.0225109028945209</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -1982,25 +1982,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.91600227134157</v>
+        <v>-1.95308165608033</v>
       </c>
       <c r="F21" t="n">
-        <v>0.257928758189887</v>
+        <v>0.235764186065949</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.139560850406393</v>
+        <v>-0.127807148941032</v>
       </c>
       <c r="H21" t="n">
-        <v>0.105925170492656</v>
+        <v>0.128157101154197</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0665272443013772</v>
+        <v>0.0555847514313396</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0112201417438982</v>
+        <v>0.016424242576247</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0112609082153799</v>
+        <v>-0.014699123668472</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -2020,25 +2020,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>-2.61515646363081</v>
+        <v>-2.70892943143692</v>
       </c>
       <c r="F22" t="n">
-        <v>0.320756770614934</v>
+        <v>0.395908632478748</v>
       </c>
       <c r="G22" t="n">
-        <v>0.213278475676705</v>
+        <v>0.242382907798554</v>
       </c>
       <c r="H22" t="n">
-        <v>0.172728878584829</v>
+        <v>0.219530970391322</v>
       </c>
       <c r="I22" t="n">
-        <v>0.102884905895322</v>
+        <v>0.156743645271192</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0298352654971725</v>
+        <v>0.0481938469609553</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0348334841073863</v>
+        <v>-0.0662510125415888</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>
@@ -2051,12 +2051,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -2110,25 +2110,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>1.97970353858253</v>
+        <v>2.03645638169679</v>
       </c>
       <c r="F2" t="n">
-        <v>0.145690465580844</v>
+        <v>0.152717764270313</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.12832256940951</v>
+        <v>-1.12190166059483</v>
       </c>
       <c r="H2" t="n">
-        <v>0.103194604784936</v>
+        <v>0.0867906653867666</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0212257117611632</v>
+        <v>0.0233227155237229</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0106491264567192</v>
+        <v>0.00753261959827769</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.0124958410297487</v>
+        <v>-0.0107506639965146</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -2148,25 +2148,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>1.93563637872471</v>
+        <v>2.0046720337807</v>
       </c>
       <c r="F3" t="n">
-        <v>0.121436695299748</v>
+        <v>0.150216926418198</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.991804474991053</v>
+        <v>-0.992824174200785</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0583512054430059</v>
+        <v>0.0678852275553906</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0147468709653237</v>
+        <v>0.0225651249825304</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00340486317665188</v>
+        <v>0.00460840412024716</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.00444446528904442</v>
+        <v>-0.00802013418412126</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -2186,25 +2186,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>2.46833408038063</v>
+        <v>2.51392827451678</v>
       </c>
       <c r="F4" t="n">
-        <v>0.22714291112948</v>
+        <v>0.201082049136534</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.03846010749416</v>
+        <v>-1.04507703041139</v>
       </c>
       <c r="H4" t="n">
-        <v>0.115243977650148</v>
+        <v>0.11006605620096</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0515939020763749</v>
+        <v>0.0404339904849474</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0132811743846279</v>
+        <v>0.0121145367276329</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.0232637853881486</v>
+        <v>-0.0187037178595124</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -2224,25 +2224,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>2.81382207634397</v>
+        <v>2.90225813456849</v>
       </c>
       <c r="F5" t="n">
-        <v>0.242498989040528</v>
+        <v>0.237300586670161</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.1205857261163</v>
+        <v>-1.14817099226754</v>
       </c>
       <c r="H5" t="n">
-        <v>0.101912722996449</v>
+        <v>0.105467977729247</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0588057596856783</v>
+        <v>0.0563115684340025</v>
       </c>
       <c r="J5" t="n">
-        <v>0.010386203108551</v>
+        <v>0.0111234943262969</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.021909225552673</v>
+        <v>-0.021248020735707</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -2262,25 +2262,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>2.01849548600067</v>
+        <v>2.08586326373053</v>
       </c>
       <c r="F6" t="n">
-        <v>0.122883242611463</v>
+        <v>0.145302181619435</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.01997434819274</v>
+        <v>-1.03120411829495</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0818857483036436</v>
+        <v>0.074283046751274</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0151002913147078</v>
+        <v>0.0211127239833672</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00670527577524767</v>
+        <v>0.00551797103465195</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.00742396882898494</v>
+        <v>-0.00869402226637252</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -2300,25 +2300,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>2.3420142874128</v>
+        <v>2.37960527088054</v>
       </c>
       <c r="F7" t="n">
-        <v>0.215810175558297</v>
+        <v>0.179786460979122</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.08629849598012</v>
+        <v>-1.07901445539707</v>
       </c>
       <c r="H7" t="n">
-        <v>0.13211005024603</v>
+        <v>0.10031066104669</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0465740318745031</v>
+        <v>0.0323231715513972</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0174530653760086</v>
+        <v>0.010062228719624</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0269241863120591</v>
+        <v>-0.0162601111896603</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -2338,25 +2338,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>1.52982703612423</v>
+        <v>1.52166620795309</v>
       </c>
       <c r="F8" t="n">
-        <v>0.343917875306103</v>
+        <v>0.333572687350795</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.830115526445352</v>
+        <v>-0.773932916603465</v>
       </c>
       <c r="H8" t="n">
-        <v>0.186708829854108</v>
+        <v>0.135974053392742</v>
       </c>
       <c r="I8" t="n">
-        <v>0.118279504955064</v>
+        <v>0.111270737746431</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0348601871454903</v>
+        <v>0.0184889431960524</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0477083810907798</v>
+        <v>-0.0303399210140507</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -2376,25 +2376,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>2.4381676875878</v>
+        <v>2.48739055832804</v>
       </c>
       <c r="F9" t="n">
-        <v>0.484812865854487</v>
+        <v>0.423446230224185</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.07201620635763</v>
+        <v>-1.07834058869686</v>
       </c>
       <c r="H9" t="n">
-        <v>0.192364462982496</v>
+        <v>0.159202180743191</v>
       </c>
       <c r="I9" t="n">
-        <v>0.235043514898041</v>
+        <v>0.179306709891073</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0370040866185441</v>
+        <v>0.0253453343533878</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0878022120874772</v>
+        <v>-0.0627180539399422</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -2414,25 +2414,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>1.41853795862842</v>
+        <v>1.49818030642701</v>
       </c>
       <c r="F10" t="n">
-        <v>0.298670614418002</v>
+        <v>0.331222567339514</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.997272275177952</v>
+        <v>-1.01418267661033</v>
       </c>
       <c r="H10" t="n">
-        <v>0.129046366793532</v>
+        <v>0.147453826849644</v>
       </c>
       <c r="I10" t="n">
-        <v>0.089204135916827</v>
+        <v>0.109708389114979</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0166529647826108</v>
+        <v>0.0217426310526049</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0321888868121076</v>
+        <v>-0.0418133861145634</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -2452,25 +2452,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>1.91397156346093</v>
+        <v>2.01754446692552</v>
       </c>
       <c r="F11" t="n">
-        <v>0.251259573281716</v>
+        <v>0.317384281227654</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.965044938060798</v>
+        <v>-0.984930211873869</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0796827302863566</v>
+        <v>0.101801443691546</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0631313731657098</v>
+        <v>0.100732781970394</v>
       </c>
       <c r="J11" t="n">
-        <v>0.00634933750588825</v>
+        <v>0.010363533937683</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.0158753027847061</v>
+        <v>-0.0284881700528722</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -2490,25 +2490,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>1.98537693246169</v>
+        <v>2.02696016167979</v>
       </c>
       <c r="F12" t="n">
-        <v>0.309598793339315</v>
+        <v>0.409698626967328</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.971956116966394</v>
+        <v>-0.968032021305164</v>
       </c>
       <c r="H12" t="n">
-        <v>0.12666401900976</v>
+        <v>0.161971004464799</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0958514128371598</v>
+        <v>0.167852964938914</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0160437737117049</v>
+        <v>0.026234606287336</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0289126257453649</v>
+        <v>-0.0587283707432745</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -2528,25 +2528,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>2.81513530583061</v>
+        <v>2.88150849650292</v>
       </c>
       <c r="F13" t="n">
-        <v>0.549529613637574</v>
+        <v>0.698101806909137</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.03564365282378</v>
+        <v>-1.04537780645883</v>
       </c>
       <c r="H13" t="n">
-        <v>0.177278779745409</v>
+        <v>0.221833270937624</v>
       </c>
       <c r="I13" t="n">
-        <v>0.301982796264662</v>
+        <v>0.487346132809803</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0314277657480212</v>
+        <v>0.0492100000948854</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0905067219448786</v>
+        <v>-0.149652715148843</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -2566,25 +2566,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>2.20329872621066</v>
+        <v>2.24237244057441</v>
       </c>
       <c r="F14" t="n">
-        <v>0.251472192731928</v>
+        <v>0.209726581516632</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.949589611386702</v>
+        <v>-0.947676440017259</v>
       </c>
       <c r="H14" t="n">
-        <v>0.120483913853294</v>
+        <v>0.093789380646873</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0632382637174039</v>
+        <v>0.0439852389946526</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0145163734974079</v>
+        <v>0.00879644792212403</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.0269335727041458</v>
+        <v>-0.0161834686181826</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -2604,25 +2604,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>2.40219799434963</v>
+        <v>2.46094374220508</v>
       </c>
       <c r="F15" t="n">
-        <v>0.234519749464493</v>
+        <v>0.264036571292589</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.00901173307717</v>
+        <v>-1.01546611467525</v>
       </c>
       <c r="H15" t="n">
-        <v>0.102287905033608</v>
+        <v>0.109562714690895</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0549995128888884</v>
+        <v>0.0697153109799464</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0104628155161643</v>
+        <v>0.0120039884504384</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.0211596960556413</v>
+        <v>-0.0254842257230339</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -2642,25 +2642,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>2.20170535405669</v>
+        <v>2.25444620048039</v>
       </c>
       <c r="F16" t="n">
-        <v>0.21892158455339</v>
+        <v>0.222341048830984</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.902310598510134</v>
+        <v>-0.911033282332893</v>
       </c>
       <c r="H16" t="n">
-        <v>0.114508545878668</v>
+        <v>0.102491288079624</v>
       </c>
       <c r="I16" t="n">
-        <v>0.047926660183367</v>
+        <v>0.0494355419952621</v>
       </c>
       <c r="J16" t="n">
-        <v>0.013112207079247</v>
+        <v>0.0105044641322206</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.0217737793079823</v>
+        <v>-0.0192375999914305</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -2680,25 +2680,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>0.999415283650382</v>
+        <v>0.996763855679523</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0710460548893685</v>
+        <v>0.0838183464811693</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.710160646468684</v>
+        <v>-0.717453756337411</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0371536156696288</v>
+        <v>0.0396326427899414</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00504754191534316</v>
+        <v>0.00702551520683735</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00138039115732648</v>
+        <v>0.00157074637451509</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.00121965787689204</v>
+        <v>-0.000964577313751146</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -2718,25 +2718,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>1.13237362326564</v>
+        <v>1.12639172344645</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0882260712790033</v>
+        <v>0.105907986747605</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.691559258068776</v>
+        <v>-0.699866140753643</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0375498739940975</v>
+        <v>0.0462881852377329</v>
       </c>
       <c r="I18" t="n">
-        <v>0.00778383965332777</v>
+        <v>0.0112165016569309</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0014099930369726</v>
+        <v>0.00214259609260268</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.00251196077708807</v>
+        <v>-0.00303414204430054</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -2756,25 +2756,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>2.25372991308615</v>
+        <v>2.30823999869546</v>
       </c>
       <c r="F19" t="n">
-        <v>0.193599458785533</v>
+        <v>0.212100236552518</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.05166003595957</v>
+        <v>-1.06317174036088</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0926540495239974</v>
+        <v>0.0883723508302685</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0374807504420513</v>
+        <v>0.0449865103456341</v>
       </c>
       <c r="J19" t="n">
-        <v>0.00858477289319537</v>
+        <v>0.00780967239126806</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0159888332730207</v>
+        <v>-0.0158401672908242</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -2794,25 +2794,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>2.29516138426015</v>
+        <v>2.39272083727114</v>
       </c>
       <c r="F20" t="n">
-        <v>0.222364136608754</v>
+        <v>0.265967582835733</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.17781611095422</v>
+        <v>-1.21578962659053</v>
       </c>
       <c r="H20" t="n">
-        <v>0.104923760248021</v>
+        <v>0.119222995723348</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0494458092497564</v>
+        <v>0.0707387551194827</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0110089954645841</v>
+        <v>0.0142141227092495</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0206429316639446</v>
+        <v>-0.0289436015331549</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -2832,25 +2832,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>1.02869503297525</v>
+        <v>1.05257362849532</v>
       </c>
       <c r="F21" t="n">
-        <v>0.265769224642769</v>
+        <v>0.288080901041177</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.717688599529452</v>
+        <v>-0.717436925236619</v>
       </c>
       <c r="H21" t="n">
-        <v>0.103533830249769</v>
+        <v>0.124537607141585</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0706332807672187</v>
+        <v>0.0829906055446962</v>
       </c>
       <c r="J21" t="n">
-        <v>0.010719254006188</v>
+        <v>0.0155096155925518</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0171998828454053</v>
+        <v>-0.0278016389585685</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -2870,25 +2870,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>1.85768941713106</v>
+        <v>1.89257104125165</v>
       </c>
       <c r="F22" t="n">
-        <v>0.336969112651298</v>
+        <v>0.410670123606949</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.993295258875856</v>
+        <v>-0.987198951461175</v>
       </c>
       <c r="H22" t="n">
-        <v>0.157840161947571</v>
+        <v>0.173663665314817</v>
       </c>
       <c r="I22" t="n">
-        <v>0.113548182881003</v>
+        <v>0.168649950423347</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0249135167236354</v>
+        <v>0.0301590686505767</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0414908144906914</v>
+        <v>-0.0611261870872031</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>
@@ -2901,12 +2901,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -2960,25 +2960,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.72519678835276</v>
+        <v>-1.777951348557</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0869111420140341</v>
+        <v>0.0825379900743899</v>
       </c>
       <c r="G2" t="n">
-        <v>1.99546287416998</v>
+        <v>0.679424176932772</v>
       </c>
       <c r="H2" t="n">
-        <v>0.204557243415721</v>
+        <v>0.0853173482110215</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00755354660618361</v>
+        <v>0.00681251980552008</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0418436658338387</v>
+        <v>0.00727904990576069</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00949575258569563</v>
+        <v>0.00220984086502586</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -2998,25 +2998,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.93060133863177</v>
+        <v>-1.99340653773269</v>
       </c>
       <c r="F3" t="n">
-        <v>0.102811464864021</v>
+        <v>0.0976327313995331</v>
       </c>
       <c r="G3" t="n">
-        <v>1.71540910960479</v>
+        <v>0.535253073568705</v>
       </c>
       <c r="H3" t="n">
-        <v>0.128615701649951</v>
+        <v>0.0774279575833975</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0105701973074859</v>
+        <v>0.00953215024053337</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0165419987109093</v>
+        <v>0.00599508861553641</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00506328286632033</v>
+        <v>0.0017118540801892</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -3036,25 +3036,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.3370003112681</v>
+        <v>-2.36474220234867</v>
       </c>
       <c r="F4" t="n">
-        <v>0.129544185691206</v>
+        <v>0.137854567634377</v>
       </c>
       <c r="G4" t="n">
-        <v>1.73953940198937</v>
+        <v>0.55764737964053</v>
       </c>
       <c r="H4" t="n">
-        <v>0.208695357802345</v>
+        <v>0.111678500072081</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0167816960463977</v>
+        <v>0.019003881817661</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0435537523682489</v>
+        <v>0.0124720873783497</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0130353650991837</v>
+        <v>0.00905882053789058</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -3074,25 +3074,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.48934273642372</v>
+        <v>-2.5105798322056</v>
       </c>
       <c r="F5" t="n">
-        <v>0.116141918019508</v>
+        <v>0.127186380028304</v>
       </c>
       <c r="G5" t="n">
-        <v>1.86641737773398</v>
+        <v>0.647579535658755</v>
       </c>
       <c r="H5" t="n">
-        <v>0.18441970056748</v>
+        <v>0.0977150205592001</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0134889451212501</v>
+        <v>0.0161763752647042</v>
       </c>
       <c r="J5" t="n">
-        <v>0.034010625957399</v>
+        <v>0.00954822524288489</v>
       </c>
       <c r="K5" t="n">
-        <v>0.00574248268227631</v>
+        <v>0.00484636394239416</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -3112,25 +3112,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.94481970743779</v>
+        <v>-1.98994626729784</v>
       </c>
       <c r="F6" t="n">
-        <v>0.105783665680401</v>
+        <v>0.0920141316934637</v>
       </c>
       <c r="G6" t="n">
-        <v>1.78244840612281</v>
+        <v>0.582431980739211</v>
       </c>
       <c r="H6" t="n">
-        <v>0.145920306625554</v>
+        <v>0.0716241750542441</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0111901839247827</v>
+        <v>0.00846660043130209</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0212927358856957</v>
+        <v>0.00513002245220101</v>
       </c>
       <c r="K6" t="n">
-        <v>0.00854226654679157</v>
+        <v>0.00154409368478559</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -3150,25 +3150,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.08438385665272</v>
+        <v>-2.12776853505119</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0833283834066869</v>
+        <v>0.0802505639146212</v>
       </c>
       <c r="G7" t="n">
-        <v>2.00821523370502</v>
+        <v>0.682229582156072</v>
       </c>
       <c r="H7" t="n">
-        <v>0.264693199286976</v>
+        <v>0.102850940330416</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00694361948117181</v>
+        <v>0.0064401530086147</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0700624897487748</v>
+        <v>0.0105783159268507</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01381622202849</v>
+        <v>0.00421831753931453</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -3188,25 +3188,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.83920081528535</v>
+        <v>-1.9482535140164</v>
       </c>
       <c r="F8" t="n">
-        <v>0.283458625754857</v>
+        <v>0.320334372530899</v>
       </c>
       <c r="G8" t="n">
-        <v>1.43323566724509</v>
+        <v>0.261024068593365</v>
       </c>
       <c r="H8" t="n">
-        <v>0.380173870798206</v>
+        <v>0.189629506963794</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0803487925148324</v>
+        <v>0.102614110224765</v>
       </c>
       <c r="J8" t="n">
-        <v>0.144532172037691</v>
+        <v>0.0359593499113315</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0219698548481498</v>
+        <v>0.00923537545251059</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -3226,25 +3226,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.28588536418224</v>
+        <v>-2.3202820840382</v>
       </c>
       <c r="F9" t="n">
-        <v>0.118148159030896</v>
+        <v>0.12396398295321</v>
       </c>
       <c r="G9" t="n">
-        <v>1.97834259892908</v>
+        <v>0.686335169404983</v>
       </c>
       <c r="H9" t="n">
-        <v>0.38226490490551</v>
+        <v>0.16539975502107</v>
       </c>
       <c r="I9" t="n">
-        <v>0.01395898748239</v>
+        <v>0.0153670690696236</v>
       </c>
       <c r="J9" t="n">
-        <v>0.146126457522419</v>
+        <v>0.02735707896103</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.00159880999586965</v>
+        <v>-0.00232816030093871</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -3264,25 +3264,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.45210266844635</v>
+        <v>-1.51780137431937</v>
       </c>
       <c r="F10" t="n">
-        <v>0.163509255779092</v>
+        <v>0.174083053785454</v>
       </c>
       <c r="G10" t="n">
-        <v>1.76506582427408</v>
+        <v>0.580710717024211</v>
       </c>
       <c r="H10" t="n">
-        <v>0.238246846292879</v>
+        <v>0.149819611981135</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0267352767254325</v>
+        <v>0.0303049096152694</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0567615597685027</v>
+        <v>0.0224459161341779</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0101279729218984</v>
+        <v>-0.0072368232351397</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -3302,25 +3302,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.0339517655342</v>
+        <v>-2.1068711084345</v>
       </c>
       <c r="F11" t="n">
-        <v>0.179930231478184</v>
+        <v>0.179161935426299</v>
       </c>
       <c r="G11" t="n">
-        <v>1.64617655510194</v>
+        <v>0.523639577340592</v>
       </c>
       <c r="H11" t="n">
-        <v>0.157352972748654</v>
+        <v>0.11890355424349</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0323748881997928</v>
+        <v>0.0320989991056973</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0247599580328386</v>
+        <v>0.0141380552117345</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.00937185231836174</v>
+        <v>-0.00954686235042087</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -3340,25 +3340,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.07102831617382</v>
+        <v>-2.12000443797963</v>
       </c>
       <c r="F12" t="n">
-        <v>0.21136996067186</v>
+        <v>0.195730672493874</v>
       </c>
       <c r="G12" t="n">
-        <v>1.68163101716978</v>
+        <v>0.506820763389294</v>
       </c>
       <c r="H12" t="n">
-        <v>0.224759741543284</v>
+        <v>0.170291094817232</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0446772602744237</v>
+        <v>0.0383104961549042</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0505169414186039</v>
+        <v>0.0289990569740515</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00891023701979488</v>
+        <v>-0.00378819639480207</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -3378,25 +3378,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>-2.76933170304976</v>
+        <v>-2.79988513554914</v>
       </c>
       <c r="F13" t="n">
-        <v>0.177956593636583</v>
+        <v>0.164643636088581</v>
       </c>
       <c r="G13" t="n">
-        <v>1.91020861268176</v>
+        <v>0.629808504017636</v>
       </c>
       <c r="H13" t="n">
-        <v>0.371607190811063</v>
+        <v>0.206972626700285</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0316685492187359</v>
+        <v>0.0271075269044691</v>
       </c>
       <c r="J13" t="n">
-        <v>0.13809190426249</v>
+        <v>0.0428376682032157</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.0048304199862856</v>
+        <v>-0.00816904122751264</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -3416,25 +3416,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>-2.29189352078826</v>
+        <v>-2.33221811018217</v>
       </c>
       <c r="F14" t="n">
-        <v>0.134661724775328</v>
+        <v>0.13146167929006</v>
       </c>
       <c r="G14" t="n">
-        <v>1.63959728057625</v>
+        <v>0.487257647581758</v>
       </c>
       <c r="H14" t="n">
-        <v>0.243901739439504</v>
+        <v>0.110417509134753</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0181337801194661</v>
+        <v>0.0172821731217626</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0594880585016157</v>
+        <v>0.0121920263235233</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0106255584561674</v>
+        <v>0.00414207079880718</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -3454,25 +3454,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.35918673923445</v>
+        <v>-2.40113898532518</v>
       </c>
       <c r="F15" t="n">
-        <v>0.116437894083279</v>
+        <v>0.122189329723341</v>
       </c>
       <c r="G15" t="n">
-        <v>1.75657302549737</v>
+        <v>0.565964498875003</v>
       </c>
       <c r="H15" t="n">
-        <v>0.210949146448444</v>
+        <v>0.112695489584321</v>
       </c>
       <c r="I15" t="n">
-        <v>0.013557783178549</v>
+        <v>0.0149302322982393</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0444995423873269</v>
+        <v>0.0127002733726498</v>
       </c>
       <c r="K15" t="n">
-        <v>0.00663085164219347</v>
+        <v>0.00300575235300295</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -3492,25 +3492,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.38452510033337</v>
+        <v>-2.4143783123601</v>
       </c>
       <c r="F16" t="n">
-        <v>0.149022890586942</v>
+        <v>0.137942025672175</v>
       </c>
       <c r="G16" t="n">
-        <v>1.58591775413186</v>
+        <v>0.462959154088631</v>
       </c>
       <c r="H16" t="n">
-        <v>0.246475210808504</v>
+        <v>0.128537936727382</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0222078219188878</v>
+        <v>0.0190280024465431</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0607500295430965</v>
+        <v>0.0165220011781323</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0211604529847967</v>
+        <v>0.00808717390768899</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -3530,25 +3530,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.37351061111828</v>
+        <v>-1.35404457784318</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0975451183537697</v>
+        <v>0.128536016420039</v>
       </c>
       <c r="G17" t="n">
-        <v>1.17954533219363</v>
+        <v>0.175614504858684</v>
       </c>
       <c r="H17" t="n">
-        <v>0.064612489657263</v>
+        <v>0.0605189546240113</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00951505011465093</v>
+        <v>0.0165215075171325</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00417477381970992</v>
+        <v>0.00366254386878314</v>
       </c>
       <c r="K17" t="n">
-        <v>0.00140889801365611</v>
+        <v>0.0023704957571454</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -3568,25 +3568,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.64016821659955</v>
+        <v>-1.61323348320391</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0855002121713666</v>
+        <v>0.121792974479335</v>
       </c>
       <c r="G18" t="n">
-        <v>1.1820943127845</v>
+        <v>0.180586724304846</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0656643713394952</v>
+        <v>0.0673717463977423</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0073102862813487</v>
+        <v>0.0148335286325239</v>
       </c>
       <c r="J18" t="n">
-        <v>0.00431180966341111</v>
+        <v>0.0045389522126817</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.000502977650851661</v>
+        <v>0.00101856287708708</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -3606,25 +3606,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.14081736529117</v>
+        <v>-2.16821355133828</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0953969328983439</v>
+        <v>0.108395064222108</v>
       </c>
       <c r="G19" t="n">
-        <v>1.80317848000473</v>
+        <v>0.599206094165685</v>
       </c>
       <c r="H19" t="n">
-        <v>0.177904693938904</v>
+        <v>0.0902889678466502</v>
       </c>
       <c r="I19" t="n">
-        <v>0.00910057480641112</v>
+        <v>0.0117494899477149</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0316500801254951</v>
+        <v>0.00815209771481344</v>
       </c>
       <c r="K19" t="n">
-        <v>0.00299024922680052</v>
+        <v>0.000589220943448199</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -3644,25 +3644,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.97028949193194</v>
+        <v>-1.99064811632014</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0801902518794047</v>
+        <v>0.0821751582283421</v>
       </c>
       <c r="G20" t="n">
-        <v>2.12084194642728</v>
+        <v>0.785020862239596</v>
       </c>
       <c r="H20" t="n">
-        <v>0.213035641702335</v>
+        <v>0.106565176953077</v>
       </c>
       <c r="I20" t="n">
-        <v>0.00643047649648237</v>
+        <v>0.00675275662985306</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0453841846355257</v>
+        <v>0.0113561369390407</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.00257506918792403</v>
+        <v>-0.00158573335259087</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -3682,25 +3682,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.46716693033476</v>
+        <v>-1.50596150897498</v>
       </c>
       <c r="F21" t="n">
-        <v>0.287705749115125</v>
+        <v>0.249752256684582</v>
       </c>
       <c r="G21" t="n">
-        <v>1.26059972867232</v>
+        <v>0.222267720042517</v>
       </c>
       <c r="H21" t="n">
-        <v>0.170502953872554</v>
+        <v>0.166463011139801</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0827745980738954</v>
+        <v>0.0623761897190414</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0290712572792663</v>
+        <v>0.0277099340777296</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0044798074636298</v>
+        <v>-0.00515070683471067</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -3720,25 +3720,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>-1.89524984654235</v>
+        <v>-1.94606176905585</v>
       </c>
       <c r="F22" t="n">
-        <v>0.220566185666429</v>
+        <v>0.208222229400172</v>
       </c>
       <c r="G22" t="n">
-        <v>1.75319588941478</v>
+        <v>0.536281630291043</v>
       </c>
       <c r="H22" t="n">
-        <v>0.328357094076466</v>
+        <v>0.18904560480009</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0486494422594377</v>
+        <v>0.0433564968163777</v>
       </c>
       <c r="J22" t="n">
-        <v>0.107818381230341</v>
+        <v>0.0357382406942316</v>
       </c>
       <c r="K22" t="n">
-        <v>0.00702714895855935</v>
+        <v>-0.00355768253319537</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>
@@ -3751,12 +3751,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -3810,25 +3810,25 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.01765690253255</v>
+        <v>-2.08140174659871</v>
       </c>
       <c r="F2" t="n">
-        <v>0.103447449067094</v>
+        <v>0.101464536652</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.0190740131440861</v>
+        <v>-0.0180406304756775</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0138713780231997</v>
+        <v>0.012319060510442</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0107013747184891</v>
+        <v>0.0102950521980051</v>
       </c>
       <c r="J2" t="n">
-        <v>0.000192415128262507</v>
+        <v>0.000151759251859932</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.00050452431854454</v>
+        <v>-0.000601428257233394</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -3848,25 +3848,25 @@
         <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.29339372378354</v>
+        <v>-2.3636120790641</v>
       </c>
       <c r="F3" t="n">
-        <v>0.132301106530333</v>
+        <v>0.126087808930259</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.013784129933345</v>
+        <v>-0.0125577421591243</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00673971626319614</v>
+        <v>0.00856252069692879</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0175035827891505</v>
+        <v>0.0158981355608334</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0000454237753083905</v>
+        <v>0.0000733167606853339</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.00054132285507576</v>
+        <v>-0.000677055669639301</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -3886,25 +3886,25 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.66618220861419</v>
+        <v>-2.70193626478097</v>
       </c>
       <c r="F4" t="n">
-        <v>0.144808633201942</v>
+        <v>0.156444834207228</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0198690908444268</v>
+        <v>-0.0190879804587354</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0191775399753587</v>
+        <v>0.019550634465166</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0209695402498145</v>
+        <v>0.0244749861501269</v>
       </c>
       <c r="J4" t="n">
-        <v>0.00036777803950648</v>
+        <v>0.000382227307990537</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.00167073607669963</v>
+        <v>-0.00172192507099017</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -3924,25 +3924,25 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>-3.00530460641232</v>
+        <v>-3.06419331756653</v>
       </c>
       <c r="F5" t="n">
-        <v>0.175142582567864</v>
+        <v>0.185570645347155</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00745643115831869</v>
+        <v>0.0121285462350868</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0142202203186205</v>
+        <v>0.0163362747356503</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0306749242285411</v>
+        <v>0.0344364644145594</v>
       </c>
       <c r="J5" t="n">
-        <v>0.000202214665910108</v>
+        <v>0.000266873872238646</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.00183131118844048</v>
+        <v>-0.00195349293902929</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -3962,25 +3962,25 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.17249190145231</v>
+        <v>-2.23135235698007</v>
       </c>
       <c r="F6" t="n">
-        <v>0.111546443989113</v>
+        <v>0.101177196866545</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.0268888286602143</v>
+        <v>-0.0235283723645498</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00923898580002034</v>
+        <v>0.00996964691214282</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0124426091666163</v>
+        <v>0.0102368251657716</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0000853588586129775</v>
+        <v>0.0000993938595527989</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.000441079631820998</v>
+        <v>-0.000595977887148311</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -4000,25 +4000,25 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.25929198323504</v>
+        <v>-2.30353901599517</v>
       </c>
       <c r="F7" t="n">
-        <v>0.08253900642319</v>
+        <v>0.0849990247310865</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.0299328683024798</v>
+        <v>-0.0295289955002821</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0095122801950541</v>
+        <v>0.00740228834920616</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0068126875813274</v>
+        <v>0.00722483420523586</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0000904834745092185</v>
+        <v>0.0000547938728047933</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.000146717072827743</v>
+        <v>-0.000207469315286281</v>
       </c>
       <c r="L7" t="n">
         <v>2</v>
@@ -4038,25 +4038,25 @@
         <v>12</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.15271197631863</v>
+        <v>-2.2271083115886</v>
       </c>
       <c r="F8" t="n">
-        <v>0.295240845282059</v>
+        <v>0.34245155985288</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0312207305439134</v>
+        <v>-0.0377432470081011</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0287361000618847</v>
+        <v>0.030834685943283</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0871671567228649</v>
+        <v>0.117273070845671</v>
       </c>
       <c r="J8" t="n">
-        <v>0.000825763446766651</v>
+        <v>0.000950777857220891</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.00352109315215479</v>
+        <v>-0.00652736343257616</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -4076,25 +4076,25 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.65027185824501</v>
+        <v>-2.65972894717063</v>
       </c>
       <c r="F9" t="n">
-        <v>0.225090686544683</v>
+        <v>0.189263107546043</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00000447698641238702</v>
+        <v>-0.00246882176944569</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0270325818460841</v>
+        <v>0.0180428086912718</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0506658171691567</v>
+        <v>0.0358205238779849</v>
       </c>
       <c r="J9" t="n">
-        <v>0.000730760481265237</v>
+        <v>0.000325542945469833</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.00415997704233024</v>
+        <v>-0.00230345389205733</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -4114,25 +4114,25 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.9226526959951</v>
+        <v>-2.02381715538323</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2434248993688</v>
+        <v>0.255778640267797</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0148059705014051</v>
+        <v>0.0255597996111659</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0463504303092982</v>
+        <v>0.0404981984260776</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0592556816327103</v>
+        <v>0.0654227128172429</v>
       </c>
       <c r="J10" t="n">
-        <v>0.00214836238985711</v>
+        <v>0.00164010407575795</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.00869296177512084</v>
+        <v>-0.00711036413780034</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
@@ -4152,25 +4152,25 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.58753790062641</v>
+        <v>-2.67178985962201</v>
       </c>
       <c r="F11" t="n">
-        <v>0.210820747593303</v>
+        <v>0.230673825428547</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0146205057425297</v>
+        <v>0.0177692748011179</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0191134696191717</v>
+        <v>0.0167409973495209</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0444453876157992</v>
+        <v>0.0532104137378396</v>
       </c>
       <c r="J11" t="n">
-        <v>0.000365324720882999</v>
+        <v>0.000280260992256664</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.00225609370786197</v>
+        <v>-0.00252369250313782</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -4190,25 +4190,25 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.54933555186575</v>
+        <v>-2.61749017114501</v>
       </c>
       <c r="F12" t="n">
-        <v>0.249008871886208</v>
+        <v>0.28894923044443</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0102466828139336</v>
+        <v>0.0123792653404658</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0195441948683702</v>
+        <v>0.0306305115929061</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0620054182780418</v>
+        <v>0.0834916577744283</v>
       </c>
       <c r="J12" t="n">
-        <v>0.000381975553052829</v>
+        <v>0.000938228240443155</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.00214364487714964</v>
+        <v>-0.0063487416996439</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
@@ -4228,25 +4228,25 @@
         <v>15</v>
       </c>
       <c r="E13" t="n">
-        <v>-3.42672233937081</v>
+        <v>-3.46876419652843</v>
       </c>
       <c r="F13" t="n">
-        <v>0.243199656921414</v>
+        <v>0.299780689171852</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0243636821714332</v>
+        <v>0.0242905260330743</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0122956675768103</v>
+        <v>0.0184675218673625</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0591460731266934</v>
+        <v>0.0898684616003503</v>
       </c>
       <c r="J13" t="n">
-        <v>0.000151183441159423</v>
+        <v>0.000341049363921511</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.00126953734763064</v>
+        <v>-0.0041447436937204</v>
       </c>
       <c r="L13" t="n">
         <v>2</v>
@@ -4266,25 +4266,25 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>-2.49902757553759</v>
+        <v>-2.53774537520061</v>
       </c>
       <c r="F14" t="n">
-        <v>0.151796300191924</v>
+        <v>0.141652278771847</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.0260432363531547</v>
+        <v>-0.0256502815535124</v>
       </c>
       <c r="H14" t="n">
-        <v>0.012122266923568</v>
+        <v>0.0115962452167281</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0230421167519567</v>
+        <v>0.0200653680812571</v>
       </c>
       <c r="J14" t="n">
-        <v>0.000146949355366231</v>
+        <v>0.00013447290312649</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.000973927502218067</v>
+        <v>-0.000884315954813601</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -4304,25 +4304,25 @@
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>-2.60453622180521</v>
+        <v>-2.64863060347219</v>
       </c>
       <c r="F15" t="n">
-        <v>0.140775675694235</v>
+        <v>0.140374272993617</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.0179874448132232</v>
+        <v>-0.0168393407736236</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00981579720341566</v>
+        <v>0.0119133252065979</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0198177908671686</v>
+        <v>0.0197049365184865</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0000963498747385826</v>
+        <v>0.000141927317478162</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.000793480139508984</v>
+        <v>-0.000937601013814208</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -4342,25 +4342,25 @@
         <v>17</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.47257403697872</v>
+        <v>-2.51123869942539</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1067374594493</v>
+        <v>0.121563063431743</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0386901786342452</v>
+        <v>-0.0369299932610897</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00949365882628895</v>
+        <v>0.010499509130997</v>
       </c>
       <c r="I16" t="n">
-        <v>0.011392885249691</v>
+        <v>0.01477757839091</v>
       </c>
       <c r="J16" t="n">
-        <v>0.000090129557909974</v>
+        <v>0.000110239691991889</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.0000163124782557576</v>
+        <v>-0.000462489919387872</v>
       </c>
       <c r="L16" t="n">
         <v>3</v>
@@ -4380,25 +4380,25 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.59135908631409</v>
+        <v>-1.56961926885366</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0932982144745055</v>
+        <v>0.130599670361597</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.0889611671755879</v>
+        <v>-0.0906814699721602</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0166836023152949</v>
+        <v>0.0202486490166893</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00870455682413083</v>
+        <v>0.0170562738985578</v>
       </c>
       <c r="J17" t="n">
-        <v>0.000278342586214914</v>
+        <v>0.000410007787001074</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.00105036762195595</v>
+        <v>-0.00191837604648169</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
@@ -4418,25 +4418,25 @@
         <v>13</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.86178907503081</v>
+        <v>-1.84249044736258</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0914459151885326</v>
+        <v>0.127874783169237</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0646415225040878</v>
+        <v>-0.0639210532659732</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0128324640774315</v>
+        <v>0.0168349599084398</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0083623554046683</v>
+        <v>0.0163519601705793</v>
       </c>
       <c r="J18" t="n">
-        <v>0.000164672134298569</v>
+        <v>0.000283415875118776</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.00089930462489449</v>
+        <v>-0.00153860905264522</v>
       </c>
       <c r="L18" t="n">
         <v>2</v>
@@ -4456,25 +4456,25 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>-2.53105087692342</v>
+        <v>-2.56149356438312</v>
       </c>
       <c r="F19" t="n">
-        <v>0.130124689890718</v>
+        <v>0.14962558407627</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.00238000384600223</v>
+        <v>-0.00129002285038163</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0140000910362655</v>
+        <v>0.0138376768307981</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0169324349191557</v>
+        <v>0.0223878154101648</v>
       </c>
       <c r="J19" t="n">
-        <v>0.000196002549023721</v>
+        <v>0.000191481300073606</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.00125060303915194</v>
+        <v>-0.00137946959787476</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -4494,25 +4494,25 @@
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>-2.29936955689108</v>
+        <v>-2.34740021745688</v>
       </c>
       <c r="F20" t="n">
-        <v>0.105835268383319</v>
+        <v>0.126118366223994</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00178324955458855</v>
+        <v>0.00794657992825708</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0170697952170677</v>
+        <v>0.0201871014722952</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0112011040337692</v>
+        <v>0.0159058422990094</v>
       </c>
       <c r="J20" t="n">
-        <v>0.000291377908752626</v>
+        <v>0.000407519065852742</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0010767979983474</v>
+        <v>-0.0017874632243433</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -4532,25 +4532,25 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>-1.77351822022407</v>
+        <v>-1.8334625702322</v>
       </c>
       <c r="F21" t="n">
-        <v>0.320554106187069</v>
+        <v>0.270318049401206</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.0531899742245637</v>
+        <v>-0.0444484446995318</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0449845807907303</v>
+        <v>0.0368542173565487</v>
       </c>
       <c r="I21" t="n">
-        <v>0.10275493499339</v>
+        <v>0.0730718478320728</v>
       </c>
       <c r="J21" t="n">
-        <v>0.00202361250891774</v>
+        <v>0.00135823333696374</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0106890316796556</v>
+        <v>-0.00680553207578169</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
@@ -4570,25 +4570,25 @@
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>-2.39640552258822</v>
+        <v>-2.50741289770736</v>
       </c>
       <c r="F22" t="n">
-        <v>0.274374733260961</v>
+        <v>0.318208850704761</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0140410826723287</v>
+        <v>0.0248428547262417</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0322726576179848</v>
+        <v>0.047688533074933</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0752814942520235</v>
+        <v>0.101256872666845</v>
       </c>
       <c r="J22" t="n">
-        <v>0.00104152442972767</v>
+        <v>0.00227419618683898</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.00475935260339732</v>
+        <v>-0.0101235506567224</v>
       </c>
       <c r="L22" t="n">
         <v>2</v>

</xml_diff>